<commit_message>
a bunch of stuff
</commit_message>
<xml_diff>
--- a/docs/Comparison.xlsx
+++ b/docs/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\xcom2_my_tweaks\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3635B72-4BAF-480F-ADEF-62C1C42850CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E18BBE-CE55-48CE-A4FD-C2BAAAADB640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19092" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B6D18C04-5EFF-4A90-9265-84C7107E118D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B6D18C04-5EFF-4A90-9265-84C7107E118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1291,7 +1291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1401,12 +1401,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,10 +1422,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1754,28 +1744,28 @@
   <dimension ref="A1:M374"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="33.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="33.88671875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="28.44140625" style="3" customWidth="1"/>
     <col min="13" max="13" width="3" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="18"/>
+    <col min="14" max="16384" width="9.109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1789,7 +1779,7 @@
       <c r="L1" s="24"/>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" s="19" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="26"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1806,7 +1796,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="34" t="s">
         <v>234</v>
@@ -1823,7 +1813,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1860,7 +1850,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>283</v>
       </c>
@@ -1878,7 +1868,7 @@
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1890,7 +1880,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>245</v>
       </c>
@@ -1925,7 +1915,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1937,7 +1927,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>235</v>
       </c>
@@ -1972,7 +1962,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1984,7 +1974,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>286</v>
       </c>
@@ -2002,7 +1992,7 @@
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2014,7 +2004,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>282</v>
       </c>
@@ -2032,7 +2022,7 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2044,7 +2034,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="B15" s="34" t="s">
         <v>53</v>
@@ -2061,7 +2051,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -2098,7 +2088,7 @@
       </c>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="1:13" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2133,7 +2123,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2145,7 +2135,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>86</v>
       </c>
@@ -2180,7 +2170,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2192,7 +2182,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
         <v>296</v>
       </c>
@@ -2227,7 +2217,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2239,7 +2229,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="34" t="s">
         <v>345</v>
@@ -2256,7 +2246,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
       <c r="B24" s="2" t="s">
         <v>1</v>
@@ -2293,7 +2283,7 @@
       </c>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>171</v>
       </c>
@@ -2328,7 +2318,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -2341,7 +2331,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>181</v>
       </c>
@@ -2376,7 +2366,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -2389,7 +2379,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>360</v>
       </c>
@@ -2399,7 +2389,7 @@
       <c r="D29" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E29" s="38" t="s">
+      <c r="E29" s="3" t="s">
         <v>361</v>
       </c>
       <c r="F29" s="28" t="s">
@@ -2424,7 +2414,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -2437,7 +2427,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
         <v>362</v>
       </c>
@@ -2472,7 +2462,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -2485,7 +2475,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
       <c r="B33" s="34" t="s">
         <v>359</v>
@@ -2502,7 +2492,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="8"/>
     </row>
-    <row r="34" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27"/>
       <c r="B34" s="2" t="s">
         <v>1</v>
@@ -2539,7 +2529,7 @@
       </c>
       <c r="M34" s="8"/>
     </row>
-    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B35" s="12" t="s">
         <v>126</v>
       </c>
@@ -2574,7 +2564,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -2587,7 +2577,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="12" t="s">
         <v>35</v>
       </c>
@@ -2622,7 +2612,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2635,7 +2625,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
         <v>325</v>
       </c>
@@ -2670,7 +2660,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -2683,7 +2673,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27"/>
       <c r="B41" s="34" t="s">
         <v>63</v>
@@ -2700,7 +2690,7 @@
       <c r="L41" s="2"/>
       <c r="M41" s="8"/>
     </row>
-    <row r="42" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
       <c r="B42" s="2" t="s">
         <v>1</v>
@@ -2737,7 +2727,7 @@
       </c>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2772,7 +2762,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2785,7 +2775,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
         <v>113</v>
       </c>
@@ -2820,7 +2810,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2833,7 +2823,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="12" t="s">
         <v>116</v>
       </c>
@@ -2868,7 +2858,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -2881,7 +2871,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="12" t="s">
         <v>262</v>
       </c>
@@ -2916,7 +2906,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2929,7 +2919,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
         <v>307</v>
       </c>
@@ -2945,7 +2935,7 @@
       <c r="K51" s="16"/>
       <c r="L51" s="16"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2958,7 +2948,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="15" t="s">
         <v>270</v>
       </c>
@@ -2976,7 +2966,7 @@
       <c r="K53" s="16"/>
       <c r="L53" s="16"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2989,7 +2979,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="12" t="s">
         <v>272</v>
       </c>
@@ -3007,7 +2997,7 @@
       <c r="K55" s="16"/>
       <c r="L55" s="16"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -3020,7 +3010,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="12" t="s">
         <v>288</v>
       </c>
@@ -3055,7 +3045,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -3068,7 +3058,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="12" t="s">
         <v>313</v>
       </c>
@@ -3086,7 +3076,7 @@
       <c r="K59" s="16"/>
       <c r="L59" s="16"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -3099,7 +3089,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27"/>
       <c r="B61" s="34" t="s">
         <v>32</v>
@@ -3116,7 +3106,7 @@
       <c r="L61" s="2"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27"/>
       <c r="B62" s="2" t="s">
         <v>1</v>
@@ -3153,7 +3143,7 @@
       </c>
       <c r="M62" s="8"/>
     </row>
-    <row r="63" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="12" t="s">
         <v>11</v>
       </c>
@@ -3188,7 +3178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -3201,7 +3191,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="12" t="s">
         <v>152</v>
       </c>
@@ -3236,7 +3226,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -3249,7 +3239,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B67" s="14" t="s">
         <v>160</v>
       </c>
@@ -3284,7 +3274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -3297,7 +3287,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="27"/>
       <c r="B69" s="34" t="s">
         <v>74</v>
@@ -3314,7 +3304,7 @@
       <c r="L69" s="2"/>
       <c r="M69" s="8"/>
     </row>
-    <row r="70" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="27"/>
       <c r="B70" s="2" t="s">
         <v>1</v>
@@ -3351,7 +3341,7 @@
       </c>
       <c r="M70" s="8"/>
     </row>
-    <row r="71" spans="1:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="12" t="s">
         <v>43</v>
       </c>
@@ -3386,7 +3376,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -3399,7 +3389,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="12" t="s">
         <v>75</v>
       </c>
@@ -3434,7 +3424,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -3447,7 +3437,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="12" t="s">
         <v>319</v>
       </c>
@@ -3482,7 +3472,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -3495,7 +3485,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="12" t="s">
         <v>254</v>
       </c>
@@ -3530,7 +3520,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -3543,7 +3533,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="12" t="s">
         <v>275</v>
       </c>
@@ -3578,7 +3568,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -3591,7 +3581,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="12" t="s">
         <v>318</v>
       </c>
@@ -3609,7 +3599,7 @@
       <c r="K81" s="16"/>
       <c r="L81" s="16"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -3622,7 +3612,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="12" t="s">
         <v>311</v>
       </c>
@@ -3640,7 +3630,7 @@
       <c r="K83" s="16"/>
       <c r="L83" s="16"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -3653,7 +3643,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="27"/>
       <c r="B85" s="34" t="s">
         <v>344</v>
@@ -3670,7 +3660,7 @@
       <c r="L85" s="2"/>
       <c r="M85" s="8"/>
     </row>
-    <row r="86" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="27"/>
       <c r="B86" s="2" t="s">
         <v>1</v>
@@ -3707,7 +3697,7 @@
       </c>
       <c r="M86" s="8"/>
     </row>
-    <row r="87" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
         <v>40</v>
       </c>
@@ -3742,7 +3732,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -3755,7 +3745,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
         <v>336</v>
       </c>
@@ -3790,7 +3780,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -3803,8 +3793,8 @@
       <c r="K90" s="5"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="14" t="s">
+    <row r="91" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B91" s="36" t="s">
         <v>140</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3838,7 +3828,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -3851,8 +3841,8 @@
       <c r="K92" s="5"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B93" s="14" t="s">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B93" s="36" t="s">
         <v>150</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -3886,7 +3876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -3899,7 +3889,7 @@
       <c r="K94" s="11"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
         <v>348</v>
       </c>
@@ -3909,32 +3899,32 @@
       <c r="D95" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="36" t="s">
+      <c r="E95" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="F95" s="36" t="s">
+      <c r="F95" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G95" s="36" t="s">
+      <c r="G95" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="H95" s="36" t="s">
+      <c r="H95" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="I95" s="36" t="s">
+      <c r="I95" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="J95" s="36" t="s">
+      <c r="J95" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="K95" s="37" t="s">
+      <c r="K95" s="10" t="s">
         <v>357</v>
       </c>
       <c r="L95" s="3" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -3947,7 +3937,7 @@
       <c r="K96" s="11"/>
       <c r="L96" s="5"/>
     </row>
-    <row r="97" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="27"/>
       <c r="B97" s="34" t="s">
         <v>261</v>
@@ -3964,7 +3954,7 @@
       <c r="L97" s="2"/>
       <c r="M97" s="8"/>
     </row>
-    <row r="98" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="27"/>
       <c r="B98" s="13" t="s">
         <v>1</v>
@@ -4001,7 +3991,7 @@
       </c>
       <c r="M98" s="8"/>
     </row>
-    <row r="99" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="14" t="s">
         <v>200</v>
       </c>
@@ -4036,7 +4026,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -4049,7 +4039,7 @@
       <c r="K100" s="5"/>
       <c r="L100" s="5"/>
     </row>
-    <row r="101" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B101" s="12" t="s">
         <v>97</v>
       </c>
@@ -4084,7 +4074,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="27"/>
       <c r="B102" s="34" t="s">
         <v>96</v>
@@ -4101,7 +4091,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="8"/>
     </row>
-    <row r="103" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="27"/>
       <c r="B103" s="13" t="s">
         <v>1</v>
@@ -4138,7 +4128,7 @@
       </c>
       <c r="M103" s="8"/>
     </row>
-    <row r="104" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B104" s="12" t="s">
         <v>97</v>
       </c>
@@ -4173,7 +4163,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4186,7 +4176,7 @@
       <c r="K105" s="5"/>
       <c r="L105" s="5"/>
     </row>
-    <row r="106" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="12" t="s">
         <v>106</v>
       </c>
@@ -4221,7 +4211,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -4234,7 +4224,7 @@
       <c r="K107" s="5"/>
       <c r="L107" s="5"/>
     </row>
-    <row r="108" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="12" t="s">
         <v>221</v>
       </c>
@@ -4269,7 +4259,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -4282,7 +4272,7 @@
       <c r="K109" s="5"/>
       <c r="L109" s="5"/>
     </row>
-    <row r="110" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="12" t="s">
         <v>309</v>
       </c>
@@ -4300,7 +4290,7 @@
       <c r="K110" s="16"/>
       <c r="L110" s="16"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -4313,7 +4303,7 @@
       <c r="K111" s="5"/>
       <c r="L111" s="5"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C112" s="9"/>
       <c r="D112" s="9"/>
       <c r="F112" s="9"/>
@@ -4324,7 +4314,7 @@
       <c r="K112" s="9"/>
       <c r="L112" s="9"/>
     </row>
-    <row r="113" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
       <c r="F113" s="9"/>
@@ -4335,7 +4325,7 @@
       <c r="K113" s="9"/>
       <c r="L113" s="9"/>
     </row>
-    <row r="114" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C114" s="9"/>
       <c r="D114" s="9"/>
       <c r="F114" s="9"/>
@@ -4346,7 +4336,7 @@
       <c r="K114" s="9"/>
       <c r="L114" s="9"/>
     </row>
-    <row r="115" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C115" s="9"/>
       <c r="D115" s="9"/>
       <c r="F115" s="9"/>
@@ -4357,7 +4347,7 @@
       <c r="K115" s="9"/>
       <c r="L115" s="9"/>
     </row>
-    <row r="116" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C116" s="9"/>
       <c r="D116" s="9"/>
       <c r="F116" s="9"/>
@@ -4368,7 +4358,7 @@
       <c r="K116" s="9"/>
       <c r="L116" s="9"/>
     </row>
-    <row r="117" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C117" s="9"/>
       <c r="D117" s="9"/>
       <c r="F117" s="9"/>
@@ -4379,7 +4369,7 @@
       <c r="K117" s="9"/>
       <c r="L117" s="9"/>
     </row>
-    <row r="118" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C118" s="9"/>
       <c r="D118" s="9"/>
       <c r="F118" s="9"/>
@@ -4390,7 +4380,7 @@
       <c r="K118" s="9"/>
       <c r="L118" s="9"/>
     </row>
-    <row r="119" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
       <c r="F119" s="9"/>
@@ -4401,7 +4391,7 @@
       <c r="K119" s="9"/>
       <c r="L119" s="9"/>
     </row>
-    <row r="120" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
       <c r="F120" s="9"/>
@@ -4412,7 +4402,7 @@
       <c r="K120" s="9"/>
       <c r="L120" s="9"/>
     </row>
-    <row r="121" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C121" s="9"/>
       <c r="D121" s="9"/>
       <c r="F121" s="9"/>
@@ -4423,7 +4413,7 @@
       <c r="K121" s="9"/>
       <c r="L121" s="9"/>
     </row>
-    <row r="122" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
       <c r="F122" s="9"/>
@@ -4434,7 +4424,7 @@
       <c r="K122" s="9"/>
       <c r="L122" s="9"/>
     </row>
-    <row r="123" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C123" s="9"/>
       <c r="D123" s="9"/>
       <c r="F123" s="9"/>
@@ -4445,7 +4435,7 @@
       <c r="K123" s="9"/>
       <c r="L123" s="9"/>
     </row>
-    <row r="124" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
       <c r="F124" s="9"/>
@@ -4456,7 +4446,7 @@
       <c r="K124" s="9"/>
       <c r="L124" s="9"/>
     </row>
-    <row r="125" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C125" s="9"/>
       <c r="D125" s="9"/>
       <c r="F125" s="9"/>
@@ -4467,7 +4457,7 @@
       <c r="K125" s="9"/>
       <c r="L125" s="9"/>
     </row>
-    <row r="126" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C126" s="9"/>
       <c r="D126" s="9"/>
       <c r="F126" s="9"/>
@@ -4478,7 +4468,7 @@
       <c r="K126" s="9"/>
       <c r="L126" s="9"/>
     </row>
-    <row r="127" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
       <c r="F127" s="9"/>
@@ -4489,7 +4479,7 @@
       <c r="K127" s="9"/>
       <c r="L127" s="9"/>
     </row>
-    <row r="128" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
       <c r="F128" s="9"/>
@@ -4500,7 +4490,7 @@
       <c r="K128" s="9"/>
       <c r="L128" s="9"/>
     </row>
-    <row r="129" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
       <c r="F129" s="9"/>
@@ -4511,7 +4501,7 @@
       <c r="K129" s="9"/>
       <c r="L129" s="9"/>
     </row>
-    <row r="130" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C130" s="9"/>
       <c r="D130" s="9"/>
       <c r="F130" s="9"/>
@@ -4522,7 +4512,7 @@
       <c r="K130" s="9"/>
       <c r="L130" s="9"/>
     </row>
-    <row r="131" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C131" s="9"/>
       <c r="D131" s="9"/>
       <c r="F131" s="9"/>
@@ -4533,7 +4523,7 @@
       <c r="K131" s="9"/>
       <c r="L131" s="9"/>
     </row>
-    <row r="132" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C132" s="9"/>
       <c r="D132" s="9"/>
       <c r="F132" s="9"/>
@@ -4544,7 +4534,7 @@
       <c r="K132" s="9"/>
       <c r="L132" s="9"/>
     </row>
-    <row r="133" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C133" s="9"/>
       <c r="D133" s="9"/>
       <c r="F133" s="9"/>
@@ -4555,7 +4545,7 @@
       <c r="K133" s="9"/>
       <c r="L133" s="9"/>
     </row>
-    <row r="134" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C134" s="9"/>
       <c r="D134" s="9"/>
       <c r="F134" s="9"/>
@@ -4566,7 +4556,7 @@
       <c r="K134" s="9"/>
       <c r="L134" s="9"/>
     </row>
-    <row r="135" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C135" s="9"/>
       <c r="D135" s="9"/>
       <c r="F135" s="9"/>
@@ -4577,7 +4567,7 @@
       <c r="K135" s="9"/>
       <c r="L135" s="9"/>
     </row>
-    <row r="136" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C136" s="9"/>
       <c r="D136" s="9"/>
       <c r="F136" s="9"/>
@@ -4588,7 +4578,7 @@
       <c r="K136" s="9"/>
       <c r="L136" s="9"/>
     </row>
-    <row r="137" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C137" s="9"/>
       <c r="D137" s="9"/>
       <c r="F137" s="9"/>
@@ -4599,7 +4589,7 @@
       <c r="K137" s="9"/>
       <c r="L137" s="9"/>
     </row>
-    <row r="138" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C138" s="9"/>
       <c r="D138" s="9"/>
       <c r="F138" s="9"/>
@@ -4610,7 +4600,7 @@
       <c r="K138" s="9"/>
       <c r="L138" s="9"/>
     </row>
-    <row r="139" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C139" s="9"/>
       <c r="D139" s="9"/>
       <c r="F139" s="9"/>
@@ -4621,7 +4611,7 @@
       <c r="K139" s="9"/>
       <c r="L139" s="9"/>
     </row>
-    <row r="140" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C140" s="9"/>
       <c r="D140" s="9"/>
       <c r="F140" s="9"/>
@@ -4632,7 +4622,7 @@
       <c r="K140" s="9"/>
       <c r="L140" s="9"/>
     </row>
-    <row r="141" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C141" s="9"/>
       <c r="D141" s="9"/>
       <c r="F141" s="9"/>
@@ -4643,7 +4633,7 @@
       <c r="K141" s="9"/>
       <c r="L141" s="9"/>
     </row>
-    <row r="142" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C142" s="9"/>
       <c r="D142" s="9"/>
       <c r="F142" s="9"/>
@@ -4654,7 +4644,7 @@
       <c r="K142" s="9"/>
       <c r="L142" s="9"/>
     </row>
-    <row r="143" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C143" s="9"/>
       <c r="D143" s="9"/>
       <c r="F143" s="9"/>
@@ -4665,7 +4655,7 @@
       <c r="K143" s="9"/>
       <c r="L143" s="9"/>
     </row>
-    <row r="144" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C144" s="9"/>
       <c r="D144" s="9"/>
       <c r="F144" s="9"/>
@@ -4676,7 +4666,7 @@
       <c r="K144" s="9"/>
       <c r="L144" s="9"/>
     </row>
-    <row r="145" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C145" s="9"/>
       <c r="D145" s="9"/>
       <c r="F145" s="9"/>
@@ -4687,7 +4677,7 @@
       <c r="K145" s="9"/>
       <c r="L145" s="9"/>
     </row>
-    <row r="146" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C146" s="9"/>
       <c r="D146" s="9"/>
       <c r="F146" s="9"/>
@@ -4698,7 +4688,7 @@
       <c r="K146" s="9"/>
       <c r="L146" s="9"/>
     </row>
-    <row r="147" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C147" s="9"/>
       <c r="D147" s="9"/>
       <c r="F147" s="9"/>
@@ -4709,7 +4699,7 @@
       <c r="K147" s="9"/>
       <c r="L147" s="9"/>
     </row>
-    <row r="148" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C148" s="9"/>
       <c r="D148" s="9"/>
       <c r="F148" s="9"/>
@@ -4720,7 +4710,7 @@
       <c r="K148" s="9"/>
       <c r="L148" s="9"/>
     </row>
-    <row r="149" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C149" s="9"/>
       <c r="D149" s="9"/>
       <c r="F149" s="9"/>
@@ -4731,7 +4721,7 @@
       <c r="K149" s="9"/>
       <c r="L149" s="9"/>
     </row>
-    <row r="150" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C150" s="9"/>
       <c r="D150" s="9"/>
       <c r="F150" s="9"/>
@@ -4742,7 +4732,7 @@
       <c r="K150" s="9"/>
       <c r="L150" s="9"/>
     </row>
-    <row r="151" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C151" s="9"/>
       <c r="D151" s="9"/>
       <c r="F151" s="9"/>
@@ -4753,7 +4743,7 @@
       <c r="K151" s="9"/>
       <c r="L151" s="9"/>
     </row>
-    <row r="152" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C152" s="9"/>
       <c r="D152" s="9"/>
       <c r="F152" s="9"/>
@@ -4764,7 +4754,7 @@
       <c r="K152" s="9"/>
       <c r="L152" s="9"/>
     </row>
-    <row r="153" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C153" s="9"/>
       <c r="D153" s="9"/>
       <c r="F153" s="9"/>
@@ -4775,7 +4765,7 @@
       <c r="K153" s="9"/>
       <c r="L153" s="9"/>
     </row>
-    <row r="154" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C154" s="9"/>
       <c r="D154" s="9"/>
       <c r="F154" s="9"/>
@@ -4786,7 +4776,7 @@
       <c r="K154" s="9"/>
       <c r="L154" s="9"/>
     </row>
-    <row r="155" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C155" s="9"/>
       <c r="D155" s="9"/>
       <c r="F155" s="9"/>
@@ -4797,7 +4787,7 @@
       <c r="K155" s="9"/>
       <c r="L155" s="9"/>
     </row>
-    <row r="156" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C156" s="9"/>
       <c r="D156" s="9"/>
       <c r="F156" s="9"/>
@@ -4808,7 +4798,7 @@
       <c r="K156" s="9"/>
       <c r="L156" s="9"/>
     </row>
-    <row r="157" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C157" s="9"/>
       <c r="D157" s="9"/>
       <c r="F157" s="9"/>
@@ -4819,7 +4809,7 @@
       <c r="K157" s="9"/>
       <c r="L157" s="9"/>
     </row>
-    <row r="158" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C158" s="9"/>
       <c r="D158" s="9"/>
       <c r="F158" s="9"/>
@@ -4830,7 +4820,7 @@
       <c r="K158" s="9"/>
       <c r="L158" s="9"/>
     </row>
-    <row r="159" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C159" s="9"/>
       <c r="D159" s="9"/>
       <c r="F159" s="9"/>
@@ -4841,7 +4831,7 @@
       <c r="K159" s="9"/>
       <c r="L159" s="9"/>
     </row>
-    <row r="160" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C160" s="9"/>
       <c r="D160" s="9"/>
       <c r="F160" s="9"/>
@@ -4852,7 +4842,7 @@
       <c r="K160" s="9"/>
       <c r="L160" s="9"/>
     </row>
-    <row r="161" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C161" s="9"/>
       <c r="D161" s="9"/>
       <c r="F161" s="9"/>
@@ -4863,7 +4853,7 @@
       <c r="K161" s="9"/>
       <c r="L161" s="9"/>
     </row>
-    <row r="162" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C162" s="9"/>
       <c r="D162" s="9"/>
       <c r="F162" s="9"/>
@@ -4874,7 +4864,7 @@
       <c r="K162" s="9"/>
       <c r="L162" s="9"/>
     </row>
-    <row r="163" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C163" s="9"/>
       <c r="D163" s="9"/>
       <c r="F163" s="9"/>
@@ -4885,7 +4875,7 @@
       <c r="K163" s="9"/>
       <c r="L163" s="9"/>
     </row>
-    <row r="164" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C164" s="9"/>
       <c r="D164" s="9"/>
       <c r="F164" s="9"/>
@@ -4896,7 +4886,7 @@
       <c r="K164" s="9"/>
       <c r="L164" s="9"/>
     </row>
-    <row r="165" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C165" s="9"/>
       <c r="D165" s="9"/>
       <c r="F165" s="9"/>
@@ -4907,7 +4897,7 @@
       <c r="K165" s="9"/>
       <c r="L165" s="9"/>
     </row>
-    <row r="166" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C166" s="9"/>
       <c r="D166" s="9"/>
       <c r="F166" s="9"/>
@@ -4918,7 +4908,7 @@
       <c r="K166" s="9"/>
       <c r="L166" s="9"/>
     </row>
-    <row r="167" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C167" s="9"/>
       <c r="D167" s="9"/>
       <c r="F167" s="9"/>
@@ -4929,7 +4919,7 @@
       <c r="K167" s="9"/>
       <c r="L167" s="9"/>
     </row>
-    <row r="168" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C168" s="9"/>
       <c r="D168" s="9"/>
       <c r="F168" s="9"/>
@@ -4940,7 +4930,7 @@
       <c r="K168" s="9"/>
       <c r="L168" s="9"/>
     </row>
-    <row r="169" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C169" s="9"/>
       <c r="D169" s="9"/>
       <c r="F169" s="9"/>
@@ -4951,7 +4941,7 @@
       <c r="K169" s="9"/>
       <c r="L169" s="9"/>
     </row>
-    <row r="170" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C170" s="9"/>
       <c r="D170" s="9"/>
       <c r="F170" s="9"/>
@@ -4962,7 +4952,7 @@
       <c r="K170" s="9"/>
       <c r="L170" s="9"/>
     </row>
-    <row r="171" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C171" s="9"/>
       <c r="D171" s="9"/>
       <c r="F171" s="9"/>
@@ -4973,7 +4963,7 @@
       <c r="K171" s="9"/>
       <c r="L171" s="9"/>
     </row>
-    <row r="172" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C172" s="9"/>
       <c r="D172" s="9"/>
       <c r="F172" s="9"/>
@@ -4984,7 +4974,7 @@
       <c r="K172" s="9"/>
       <c r="L172" s="9"/>
     </row>
-    <row r="173" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C173" s="9"/>
       <c r="D173" s="9"/>
       <c r="F173" s="9"/>
@@ -4995,7 +4985,7 @@
       <c r="K173" s="9"/>
       <c r="L173" s="9"/>
     </row>
-    <row r="174" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C174" s="9"/>
       <c r="D174" s="9"/>
       <c r="F174" s="9"/>
@@ -5006,7 +4996,7 @@
       <c r="K174" s="9"/>
       <c r="L174" s="9"/>
     </row>
-    <row r="175" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C175" s="9"/>
       <c r="D175" s="9"/>
       <c r="F175" s="9"/>
@@ -5017,7 +5007,7 @@
       <c r="K175" s="9"/>
       <c r="L175" s="9"/>
     </row>
-    <row r="176" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C176" s="9"/>
       <c r="D176" s="9"/>
       <c r="F176" s="9"/>
@@ -5028,7 +5018,7 @@
       <c r="K176" s="9"/>
       <c r="L176" s="9"/>
     </row>
-    <row r="177" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C177" s="9"/>
       <c r="D177" s="9"/>
       <c r="F177" s="9"/>
@@ -5039,7 +5029,7 @@
       <c r="K177" s="9"/>
       <c r="L177" s="9"/>
     </row>
-    <row r="178" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C178" s="9"/>
       <c r="D178" s="9"/>
       <c r="F178" s="9"/>
@@ -5050,7 +5040,7 @@
       <c r="K178" s="9"/>
       <c r="L178" s="9"/>
     </row>
-    <row r="179" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C179" s="9"/>
       <c r="D179" s="9"/>
       <c r="F179" s="9"/>
@@ -5061,7 +5051,7 @@
       <c r="K179" s="9"/>
       <c r="L179" s="9"/>
     </row>
-    <row r="180" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C180" s="9"/>
       <c r="D180" s="9"/>
       <c r="F180" s="9"/>
@@ -5072,7 +5062,7 @@
       <c r="K180" s="9"/>
       <c r="L180" s="9"/>
     </row>
-    <row r="181" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C181" s="9"/>
       <c r="D181" s="9"/>
       <c r="F181" s="9"/>
@@ -5083,7 +5073,7 @@
       <c r="K181" s="9"/>
       <c r="L181" s="9"/>
     </row>
-    <row r="182" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C182" s="9"/>
       <c r="D182" s="9"/>
       <c r="F182" s="9"/>
@@ -5094,7 +5084,7 @@
       <c r="K182" s="9"/>
       <c r="L182" s="9"/>
     </row>
-    <row r="183" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C183" s="9"/>
       <c r="D183" s="9"/>
       <c r="F183" s="9"/>
@@ -5105,7 +5095,7 @@
       <c r="K183" s="9"/>
       <c r="L183" s="9"/>
     </row>
-    <row r="184" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C184" s="9"/>
       <c r="D184" s="9"/>
       <c r="F184" s="9"/>
@@ -5116,7 +5106,7 @@
       <c r="K184" s="9"/>
       <c r="L184" s="9"/>
     </row>
-    <row r="185" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C185" s="9"/>
       <c r="D185" s="9"/>
       <c r="F185" s="9"/>
@@ -5127,7 +5117,7 @@
       <c r="K185" s="9"/>
       <c r="L185" s="9"/>
     </row>
-    <row r="186" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C186" s="9"/>
       <c r="D186" s="9"/>
       <c r="F186" s="9"/>
@@ -5138,7 +5128,7 @@
       <c r="K186" s="9"/>
       <c r="L186" s="9"/>
     </row>
-    <row r="187" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C187" s="9"/>
       <c r="D187" s="9"/>
       <c r="F187" s="9"/>
@@ -5149,7 +5139,7 @@
       <c r="K187" s="9"/>
       <c r="L187" s="9"/>
     </row>
-    <row r="188" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C188" s="9"/>
       <c r="D188" s="9"/>
       <c r="F188" s="9"/>
@@ -5160,7 +5150,7 @@
       <c r="K188" s="9"/>
       <c r="L188" s="9"/>
     </row>
-    <row r="189" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C189" s="9"/>
       <c r="D189" s="9"/>
       <c r="F189" s="9"/>
@@ -5171,7 +5161,7 @@
       <c r="K189" s="9"/>
       <c r="L189" s="9"/>
     </row>
-    <row r="190" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C190" s="9"/>
       <c r="D190" s="9"/>
       <c r="F190" s="9"/>
@@ -5182,7 +5172,7 @@
       <c r="K190" s="9"/>
       <c r="L190" s="9"/>
     </row>
-    <row r="191" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C191" s="9"/>
       <c r="D191" s="9"/>
       <c r="F191" s="9"/>
@@ -5193,7 +5183,7 @@
       <c r="K191" s="9"/>
       <c r="L191" s="9"/>
     </row>
-    <row r="192" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C192" s="9"/>
       <c r="D192" s="9"/>
       <c r="F192" s="9"/>
@@ -5204,7 +5194,7 @@
       <c r="K192" s="9"/>
       <c r="L192" s="9"/>
     </row>
-    <row r="193" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C193" s="9"/>
       <c r="D193" s="9"/>
       <c r="F193" s="9"/>
@@ -5215,7 +5205,7 @@
       <c r="K193" s="9"/>
       <c r="L193" s="9"/>
     </row>
-    <row r="194" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C194" s="9"/>
       <c r="D194" s="9"/>
       <c r="F194" s="9"/>
@@ -5226,7 +5216,7 @@
       <c r="K194" s="9"/>
       <c r="L194" s="9"/>
     </row>
-    <row r="195" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C195" s="9"/>
       <c r="D195" s="9"/>
       <c r="F195" s="9"/>
@@ -5237,7 +5227,7 @@
       <c r="K195" s="9"/>
       <c r="L195" s="9"/>
     </row>
-    <row r="196" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C196" s="9"/>
       <c r="D196" s="9"/>
       <c r="F196" s="9"/>
@@ -5248,7 +5238,7 @@
       <c r="K196" s="9"/>
       <c r="L196" s="9"/>
     </row>
-    <row r="197" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C197" s="9"/>
       <c r="D197" s="9"/>
       <c r="F197" s="9"/>
@@ -5259,7 +5249,7 @@
       <c r="K197" s="9"/>
       <c r="L197" s="9"/>
     </row>
-    <row r="198" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C198" s="9"/>
       <c r="D198" s="9"/>
       <c r="F198" s="9"/>
@@ -5270,7 +5260,7 @@
       <c r="K198" s="9"/>
       <c r="L198" s="9"/>
     </row>
-    <row r="199" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C199" s="9"/>
       <c r="D199" s="9"/>
       <c r="F199" s="9"/>
@@ -5281,7 +5271,7 @@
       <c r="K199" s="9"/>
       <c r="L199" s="9"/>
     </row>
-    <row r="200" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C200" s="9"/>
       <c r="D200" s="9"/>
       <c r="F200" s="9"/>
@@ -5292,7 +5282,7 @@
       <c r="K200" s="9"/>
       <c r="L200" s="9"/>
     </row>
-    <row r="201" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C201" s="9"/>
       <c r="D201" s="9"/>
       <c r="F201" s="9"/>
@@ -5303,7 +5293,7 @@
       <c r="K201" s="9"/>
       <c r="L201" s="9"/>
     </row>
-    <row r="202" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C202" s="9"/>
       <c r="D202" s="9"/>
       <c r="F202" s="9"/>
@@ -5314,7 +5304,7 @@
       <c r="K202" s="9"/>
       <c r="L202" s="9"/>
     </row>
-    <row r="203" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C203" s="9"/>
       <c r="D203" s="9"/>
       <c r="F203" s="9"/>
@@ -5325,7 +5315,7 @@
       <c r="K203" s="9"/>
       <c r="L203" s="9"/>
     </row>
-    <row r="204" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C204" s="9"/>
       <c r="D204" s="9"/>
       <c r="F204" s="9"/>
@@ -5336,7 +5326,7 @@
       <c r="K204" s="9"/>
       <c r="L204" s="9"/>
     </row>
-    <row r="205" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C205" s="9"/>
       <c r="D205" s="9"/>
       <c r="F205" s="9"/>
@@ -5347,7 +5337,7 @@
       <c r="K205" s="9"/>
       <c r="L205" s="9"/>
     </row>
-    <row r="206" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C206" s="9"/>
       <c r="D206" s="9"/>
       <c r="F206" s="9"/>
@@ -5358,7 +5348,7 @@
       <c r="K206" s="9"/>
       <c r="L206" s="9"/>
     </row>
-    <row r="207" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C207" s="9"/>
       <c r="D207" s="9"/>
       <c r="F207" s="9"/>
@@ -5369,7 +5359,7 @@
       <c r="K207" s="9"/>
       <c r="L207" s="9"/>
     </row>
-    <row r="208" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C208" s="9"/>
       <c r="D208" s="9"/>
       <c r="F208" s="9"/>
@@ -5380,7 +5370,7 @@
       <c r="K208" s="9"/>
       <c r="L208" s="9"/>
     </row>
-    <row r="209" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C209" s="9"/>
       <c r="D209" s="9"/>
       <c r="F209" s="9"/>
@@ -5391,7 +5381,7 @@
       <c r="K209" s="9"/>
       <c r="L209" s="9"/>
     </row>
-    <row r="210" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C210" s="9"/>
       <c r="D210" s="9"/>
       <c r="F210" s="9"/>
@@ -5402,7 +5392,7 @@
       <c r="K210" s="9"/>
       <c r="L210" s="9"/>
     </row>
-    <row r="211" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C211" s="9"/>
       <c r="D211" s="9"/>
       <c r="F211" s="9"/>
@@ -5413,7 +5403,7 @@
       <c r="K211" s="9"/>
       <c r="L211" s="9"/>
     </row>
-    <row r="212" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C212" s="9"/>
       <c r="D212" s="9"/>
       <c r="F212" s="9"/>
@@ -5424,7 +5414,7 @@
       <c r="K212" s="9"/>
       <c r="L212" s="9"/>
     </row>
-    <row r="213" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C213" s="9"/>
       <c r="D213" s="9"/>
       <c r="F213" s="9"/>
@@ -5435,7 +5425,7 @@
       <c r="K213" s="9"/>
       <c r="L213" s="9"/>
     </row>
-    <row r="214" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C214" s="9"/>
       <c r="D214" s="9"/>
       <c r="F214" s="9"/>
@@ -5446,7 +5436,7 @@
       <c r="K214" s="9"/>
       <c r="L214" s="9"/>
     </row>
-    <row r="215" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C215" s="9"/>
       <c r="D215" s="9"/>
       <c r="F215" s="9"/>
@@ -5457,7 +5447,7 @@
       <c r="K215" s="9"/>
       <c r="L215" s="9"/>
     </row>
-    <row r="216" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C216" s="9"/>
       <c r="D216" s="9"/>
       <c r="F216" s="9"/>
@@ -5468,7 +5458,7 @@
       <c r="K216" s="9"/>
       <c r="L216" s="9"/>
     </row>
-    <row r="217" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C217" s="9"/>
       <c r="D217" s="9"/>
       <c r="F217" s="9"/>
@@ -5479,7 +5469,7 @@
       <c r="K217" s="9"/>
       <c r="L217" s="9"/>
     </row>
-    <row r="218" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C218" s="9"/>
       <c r="D218" s="9"/>
       <c r="F218" s="9"/>
@@ -5490,7 +5480,7 @@
       <c r="K218" s="9"/>
       <c r="L218" s="9"/>
     </row>
-    <row r="219" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C219" s="9"/>
       <c r="D219" s="9"/>
       <c r="F219" s="9"/>
@@ -5501,7 +5491,7 @@
       <c r="K219" s="9"/>
       <c r="L219" s="9"/>
     </row>
-    <row r="220" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C220" s="9"/>
       <c r="D220" s="9"/>
       <c r="F220" s="9"/>
@@ -5512,7 +5502,7 @@
       <c r="K220" s="9"/>
       <c r="L220" s="9"/>
     </row>
-    <row r="221" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C221" s="9"/>
       <c r="D221" s="9"/>
       <c r="F221" s="9"/>
@@ -5523,7 +5513,7 @@
       <c r="K221" s="9"/>
       <c r="L221" s="9"/>
     </row>
-    <row r="222" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C222" s="9"/>
       <c r="D222" s="9"/>
       <c r="F222" s="9"/>
@@ -5534,7 +5524,7 @@
       <c r="K222" s="9"/>
       <c r="L222" s="9"/>
     </row>
-    <row r="223" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C223" s="9"/>
       <c r="D223" s="9"/>
       <c r="F223" s="9"/>
@@ -5545,7 +5535,7 @@
       <c r="K223" s="9"/>
       <c r="L223" s="9"/>
     </row>
-    <row r="224" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C224" s="9"/>
       <c r="D224" s="9"/>
       <c r="F224" s="9"/>
@@ -5556,7 +5546,7 @@
       <c r="K224" s="9"/>
       <c r="L224" s="9"/>
     </row>
-    <row r="225" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C225" s="9"/>
       <c r="D225" s="9"/>
       <c r="F225" s="9"/>
@@ -5567,7 +5557,7 @@
       <c r="K225" s="9"/>
       <c r="L225" s="9"/>
     </row>
-    <row r="226" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C226" s="9"/>
       <c r="D226" s="9"/>
       <c r="F226" s="9"/>
@@ -5578,7 +5568,7 @@
       <c r="K226" s="9"/>
       <c r="L226" s="9"/>
     </row>
-    <row r="227" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C227" s="9"/>
       <c r="D227" s="9"/>
       <c r="F227" s="9"/>
@@ -5589,7 +5579,7 @@
       <c r="K227" s="9"/>
       <c r="L227" s="9"/>
     </row>
-    <row r="228" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C228" s="9"/>
       <c r="D228" s="9"/>
       <c r="F228" s="9"/>
@@ -5600,7 +5590,7 @@
       <c r="K228" s="9"/>
       <c r="L228" s="9"/>
     </row>
-    <row r="229" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C229" s="9"/>
       <c r="D229" s="9"/>
       <c r="F229" s="9"/>
@@ -5611,7 +5601,7 @@
       <c r="K229" s="9"/>
       <c r="L229" s="9"/>
     </row>
-    <row r="230" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C230" s="9"/>
       <c r="D230" s="9"/>
       <c r="F230" s="9"/>
@@ -5622,7 +5612,7 @@
       <c r="K230" s="9"/>
       <c r="L230" s="9"/>
     </row>
-    <row r="231" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C231" s="9"/>
       <c r="D231" s="9"/>
       <c r="F231" s="9"/>
@@ -5633,7 +5623,7 @@
       <c r="K231" s="9"/>
       <c r="L231" s="9"/>
     </row>
-    <row r="232" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C232" s="9"/>
       <c r="D232" s="9"/>
       <c r="F232" s="9"/>
@@ -5644,7 +5634,7 @@
       <c r="K232" s="9"/>
       <c r="L232" s="9"/>
     </row>
-    <row r="233" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C233" s="9"/>
       <c r="D233" s="9"/>
       <c r="F233" s="9"/>
@@ -5655,7 +5645,7 @@
       <c r="K233" s="9"/>
       <c r="L233" s="9"/>
     </row>
-    <row r="234" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C234" s="9"/>
       <c r="D234" s="9"/>
       <c r="F234" s="9"/>
@@ -5666,7 +5656,7 @@
       <c r="K234" s="9"/>
       <c r="L234" s="9"/>
     </row>
-    <row r="235" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C235" s="9"/>
       <c r="D235" s="9"/>
       <c r="F235" s="9"/>
@@ -5677,7 +5667,7 @@
       <c r="K235" s="9"/>
       <c r="L235" s="9"/>
     </row>
-    <row r="236" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C236" s="9"/>
       <c r="D236" s="9"/>
       <c r="F236" s="9"/>
@@ -5688,7 +5678,7 @@
       <c r="K236" s="9"/>
       <c r="L236" s="9"/>
     </row>
-    <row r="237" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C237" s="9"/>
       <c r="D237" s="9"/>
       <c r="F237" s="9"/>
@@ -5699,7 +5689,7 @@
       <c r="K237" s="9"/>
       <c r="L237" s="9"/>
     </row>
-    <row r="238" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C238" s="9"/>
       <c r="D238" s="9"/>
       <c r="F238" s="9"/>
@@ -5710,7 +5700,7 @@
       <c r="K238" s="9"/>
       <c r="L238" s="9"/>
     </row>
-    <row r="239" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C239" s="9"/>
       <c r="D239" s="9"/>
       <c r="F239" s="9"/>
@@ -5721,7 +5711,7 @@
       <c r="K239" s="9"/>
       <c r="L239" s="9"/>
     </row>
-    <row r="240" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C240" s="9"/>
       <c r="D240" s="9"/>
       <c r="F240" s="9"/>
@@ -5732,7 +5722,7 @@
       <c r="K240" s="9"/>
       <c r="L240" s="9"/>
     </row>
-    <row r="241" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C241" s="9"/>
       <c r="D241" s="9"/>
       <c r="F241" s="9"/>
@@ -5743,7 +5733,7 @@
       <c r="K241" s="9"/>
       <c r="L241" s="9"/>
     </row>
-    <row r="242" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C242" s="9"/>
       <c r="D242" s="9"/>
       <c r="F242" s="9"/>
@@ -5754,7 +5744,7 @@
       <c r="K242" s="9"/>
       <c r="L242" s="9"/>
     </row>
-    <row r="243" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C243" s="9"/>
       <c r="D243" s="9"/>
       <c r="F243" s="9"/>
@@ -5765,7 +5755,7 @@
       <c r="K243" s="9"/>
       <c r="L243" s="9"/>
     </row>
-    <row r="244" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C244" s="9"/>
       <c r="D244" s="9"/>
       <c r="F244" s="9"/>
@@ -5776,7 +5766,7 @@
       <c r="K244" s="9"/>
       <c r="L244" s="9"/>
     </row>
-    <row r="245" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C245" s="9"/>
       <c r="D245" s="9"/>
       <c r="F245" s="9"/>
@@ -5787,7 +5777,7 @@
       <c r="K245" s="9"/>
       <c r="L245" s="9"/>
     </row>
-    <row r="246" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C246" s="9"/>
       <c r="D246" s="9"/>
       <c r="F246" s="9"/>
@@ -5798,7 +5788,7 @@
       <c r="K246" s="9"/>
       <c r="L246" s="9"/>
     </row>
-    <row r="247" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C247" s="9"/>
       <c r="D247" s="9"/>
       <c r="F247" s="9"/>
@@ -5809,7 +5799,7 @@
       <c r="K247" s="9"/>
       <c r="L247" s="9"/>
     </row>
-    <row r="248" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C248" s="9"/>
       <c r="D248" s="9"/>
       <c r="F248" s="9"/>
@@ -5820,7 +5810,7 @@
       <c r="K248" s="9"/>
       <c r="L248" s="9"/>
     </row>
-    <row r="249" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C249" s="9"/>
       <c r="D249" s="9"/>
       <c r="F249" s="9"/>
@@ -5831,7 +5821,7 @@
       <c r="K249" s="9"/>
       <c r="L249" s="9"/>
     </row>
-    <row r="250" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C250" s="9"/>
       <c r="D250" s="9"/>
       <c r="F250" s="9"/>
@@ -5842,7 +5832,7 @@
       <c r="K250" s="9"/>
       <c r="L250" s="9"/>
     </row>
-    <row r="251" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C251" s="9"/>
       <c r="D251" s="9"/>
       <c r="F251" s="9"/>
@@ -5853,7 +5843,7 @@
       <c r="K251" s="9"/>
       <c r="L251" s="9"/>
     </row>
-    <row r="252" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C252" s="9"/>
       <c r="D252" s="9"/>
       <c r="F252" s="9"/>
@@ -5864,7 +5854,7 @@
       <c r="K252" s="9"/>
       <c r="L252" s="9"/>
     </row>
-    <row r="253" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C253" s="9"/>
       <c r="D253" s="9"/>
       <c r="F253" s="9"/>
@@ -5875,7 +5865,7 @@
       <c r="K253" s="9"/>
       <c r="L253" s="9"/>
     </row>
-    <row r="254" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C254" s="9"/>
       <c r="D254" s="9"/>
       <c r="F254" s="9"/>
@@ -5886,7 +5876,7 @@
       <c r="K254" s="9"/>
       <c r="L254" s="9"/>
     </row>
-    <row r="255" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C255" s="9"/>
       <c r="D255" s="9"/>
       <c r="F255" s="9"/>
@@ -5897,7 +5887,7 @@
       <c r="K255" s="9"/>
       <c r="L255" s="9"/>
     </row>
-    <row r="256" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C256" s="9"/>
       <c r="D256" s="9"/>
       <c r="F256" s="9"/>
@@ -5908,7 +5898,7 @@
       <c r="K256" s="9"/>
       <c r="L256" s="9"/>
     </row>
-    <row r="257" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C257" s="9"/>
       <c r="D257" s="9"/>
       <c r="F257" s="9"/>
@@ -5919,7 +5909,7 @@
       <c r="K257" s="9"/>
       <c r="L257" s="9"/>
     </row>
-    <row r="258" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C258" s="9"/>
       <c r="D258" s="9"/>
       <c r="F258" s="9"/>
@@ -5930,7 +5920,7 @@
       <c r="K258" s="9"/>
       <c r="L258" s="9"/>
     </row>
-    <row r="259" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C259" s="9"/>
       <c r="D259" s="9"/>
       <c r="F259" s="9"/>
@@ -5941,7 +5931,7 @@
       <c r="K259" s="9"/>
       <c r="L259" s="9"/>
     </row>
-    <row r="260" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C260" s="9"/>
       <c r="D260" s="9"/>
       <c r="F260" s="9"/>
@@ -5952,7 +5942,7 @@
       <c r="K260" s="9"/>
       <c r="L260" s="9"/>
     </row>
-    <row r="261" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C261" s="9"/>
       <c r="D261" s="9"/>
       <c r="F261" s="9"/>
@@ -5963,7 +5953,7 @@
       <c r="K261" s="9"/>
       <c r="L261" s="9"/>
     </row>
-    <row r="262" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C262" s="9"/>
       <c r="D262" s="9"/>
       <c r="F262" s="9"/>
@@ -5974,7 +5964,7 @@
       <c r="K262" s="9"/>
       <c r="L262" s="9"/>
     </row>
-    <row r="263" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C263" s="9"/>
       <c r="D263" s="9"/>
       <c r="F263" s="9"/>
@@ -5985,7 +5975,7 @@
       <c r="K263" s="9"/>
       <c r="L263" s="9"/>
     </row>
-    <row r="264" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C264" s="9"/>
       <c r="D264" s="9"/>
       <c r="F264" s="9"/>
@@ -5996,7 +5986,7 @@
       <c r="K264" s="9"/>
       <c r="L264" s="9"/>
     </row>
-    <row r="265" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C265" s="9"/>
       <c r="D265" s="9"/>
       <c r="F265" s="9"/>
@@ -6007,7 +5997,7 @@
       <c r="K265" s="9"/>
       <c r="L265" s="9"/>
     </row>
-    <row r="266" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C266" s="9"/>
       <c r="D266" s="9"/>
       <c r="F266" s="9"/>
@@ -6018,7 +6008,7 @@
       <c r="K266" s="9"/>
       <c r="L266" s="9"/>
     </row>
-    <row r="267" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C267" s="9"/>
       <c r="D267" s="9"/>
       <c r="F267" s="9"/>
@@ -6029,7 +6019,7 @@
       <c r="K267" s="9"/>
       <c r="L267" s="9"/>
     </row>
-    <row r="268" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C268" s="9"/>
       <c r="D268" s="9"/>
       <c r="F268" s="9"/>
@@ -6040,7 +6030,7 @@
       <c r="K268" s="9"/>
       <c r="L268" s="9"/>
     </row>
-    <row r="269" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C269" s="9"/>
       <c r="D269" s="9"/>
       <c r="F269" s="9"/>
@@ -6051,7 +6041,7 @@
       <c r="K269" s="9"/>
       <c r="L269" s="9"/>
     </row>
-    <row r="270" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C270" s="9"/>
       <c r="D270" s="9"/>
       <c r="F270" s="9"/>
@@ -6062,7 +6052,7 @@
       <c r="K270" s="9"/>
       <c r="L270" s="9"/>
     </row>
-    <row r="271" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C271" s="9"/>
       <c r="D271" s="9"/>
       <c r="F271" s="9"/>
@@ -6073,7 +6063,7 @@
       <c r="K271" s="9"/>
       <c r="L271" s="9"/>
     </row>
-    <row r="272" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C272" s="9"/>
       <c r="D272" s="9"/>
       <c r="F272" s="9"/>
@@ -6084,7 +6074,7 @@
       <c r="K272" s="9"/>
       <c r="L272" s="9"/>
     </row>
-    <row r="273" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C273" s="9"/>
       <c r="D273" s="9"/>
       <c r="F273" s="9"/>
@@ -6095,7 +6085,7 @@
       <c r="K273" s="9"/>
       <c r="L273" s="9"/>
     </row>
-    <row r="274" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C274" s="9"/>
       <c r="D274" s="9"/>
       <c r="F274" s="9"/>
@@ -6106,7 +6096,7 @@
       <c r="K274" s="9"/>
       <c r="L274" s="9"/>
     </row>
-    <row r="275" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C275" s="9"/>
       <c r="D275" s="9"/>
       <c r="F275" s="9"/>
@@ -6117,7 +6107,7 @@
       <c r="K275" s="9"/>
       <c r="L275" s="9"/>
     </row>
-    <row r="276" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C276" s="9"/>
       <c r="D276" s="9"/>
       <c r="F276" s="9"/>
@@ -6128,7 +6118,7 @@
       <c r="K276" s="9"/>
       <c r="L276" s="9"/>
     </row>
-    <row r="277" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C277" s="9"/>
       <c r="D277" s="9"/>
       <c r="F277" s="9"/>
@@ -6139,7 +6129,7 @@
       <c r="K277" s="9"/>
       <c r="L277" s="9"/>
     </row>
-    <row r="278" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C278" s="9"/>
       <c r="D278" s="9"/>
       <c r="F278" s="9"/>
@@ -6150,7 +6140,7 @@
       <c r="K278" s="9"/>
       <c r="L278" s="9"/>
     </row>
-    <row r="279" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C279" s="9"/>
       <c r="D279" s="9"/>
       <c r="F279" s="9"/>
@@ -6161,7 +6151,7 @@
       <c r="K279" s="9"/>
       <c r="L279" s="9"/>
     </row>
-    <row r="280" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C280" s="9"/>
       <c r="D280" s="9"/>
       <c r="F280" s="9"/>
@@ -6172,7 +6162,7 @@
       <c r="K280" s="9"/>
       <c r="L280" s="9"/>
     </row>
-    <row r="281" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C281" s="9"/>
       <c r="D281" s="9"/>
       <c r="F281" s="9"/>
@@ -6183,7 +6173,7 @@
       <c r="K281" s="9"/>
       <c r="L281" s="9"/>
     </row>
-    <row r="282" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C282" s="9"/>
       <c r="D282" s="9"/>
       <c r="F282" s="9"/>
@@ -6194,7 +6184,7 @@
       <c r="K282" s="9"/>
       <c r="L282" s="9"/>
     </row>
-    <row r="283" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C283" s="9"/>
       <c r="D283" s="9"/>
       <c r="F283" s="9"/>
@@ -6205,7 +6195,7 @@
       <c r="K283" s="9"/>
       <c r="L283" s="9"/>
     </row>
-    <row r="284" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C284" s="9"/>
       <c r="D284" s="9"/>
       <c r="F284" s="9"/>
@@ -6216,7 +6206,7 @@
       <c r="K284" s="9"/>
       <c r="L284" s="9"/>
     </row>
-    <row r="285" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C285" s="9"/>
       <c r="D285" s="9"/>
       <c r="F285" s="9"/>
@@ -6227,7 +6217,7 @@
       <c r="K285" s="9"/>
       <c r="L285" s="9"/>
     </row>
-    <row r="286" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C286" s="9"/>
       <c r="D286" s="9"/>
       <c r="F286" s="9"/>
@@ -6238,7 +6228,7 @@
       <c r="K286" s="9"/>
       <c r="L286" s="9"/>
     </row>
-    <row r="287" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C287" s="9"/>
       <c r="D287" s="9"/>
       <c r="F287" s="9"/>
@@ -6249,7 +6239,7 @@
       <c r="K287" s="9"/>
       <c r="L287" s="9"/>
     </row>
-    <row r="288" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C288" s="9"/>
       <c r="D288" s="9"/>
       <c r="F288" s="9"/>
@@ -6260,7 +6250,7 @@
       <c r="K288" s="9"/>
       <c r="L288" s="9"/>
     </row>
-    <row r="289" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C289" s="9"/>
       <c r="D289" s="9"/>
       <c r="F289" s="9"/>
@@ -6271,7 +6261,7 @@
       <c r="K289" s="9"/>
       <c r="L289" s="9"/>
     </row>
-    <row r="290" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C290" s="9"/>
       <c r="D290" s="9"/>
       <c r="F290" s="9"/>
@@ -6282,7 +6272,7 @@
       <c r="K290" s="9"/>
       <c r="L290" s="9"/>
     </row>
-    <row r="291" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C291" s="9"/>
       <c r="D291" s="9"/>
       <c r="F291" s="9"/>
@@ -6293,7 +6283,7 @@
       <c r="K291" s="9"/>
       <c r="L291" s="9"/>
     </row>
-    <row r="292" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C292" s="9"/>
       <c r="D292" s="9"/>
       <c r="F292" s="9"/>
@@ -6304,7 +6294,7 @@
       <c r="K292" s="9"/>
       <c r="L292" s="9"/>
     </row>
-    <row r="293" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C293" s="9"/>
       <c r="D293" s="9"/>
       <c r="F293" s="9"/>
@@ -6315,7 +6305,7 @@
       <c r="K293" s="9"/>
       <c r="L293" s="9"/>
     </row>
-    <row r="294" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C294" s="9"/>
       <c r="D294" s="9"/>
       <c r="F294" s="9"/>
@@ -6326,7 +6316,7 @@
       <c r="K294" s="9"/>
       <c r="L294" s="9"/>
     </row>
-    <row r="295" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C295" s="9"/>
       <c r="D295" s="9"/>
       <c r="F295" s="9"/>
@@ -6337,7 +6327,7 @@
       <c r="K295" s="9"/>
       <c r="L295" s="9"/>
     </row>
-    <row r="296" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C296" s="9"/>
       <c r="D296" s="9"/>
       <c r="F296" s="9"/>
@@ -6348,7 +6338,7 @@
       <c r="K296" s="9"/>
       <c r="L296" s="9"/>
     </row>
-    <row r="297" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C297" s="9"/>
       <c r="D297" s="9"/>
       <c r="F297" s="9"/>
@@ -6359,7 +6349,7 @@
       <c r="K297" s="9"/>
       <c r="L297" s="9"/>
     </row>
-    <row r="298" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C298" s="9"/>
       <c r="D298" s="9"/>
       <c r="F298" s="9"/>
@@ -6370,7 +6360,7 @@
       <c r="K298" s="9"/>
       <c r="L298" s="9"/>
     </row>
-    <row r="299" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C299" s="9"/>
       <c r="D299" s="9"/>
       <c r="F299" s="9"/>
@@ -6381,7 +6371,7 @@
       <c r="K299" s="9"/>
       <c r="L299" s="9"/>
     </row>
-    <row r="300" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C300" s="9"/>
       <c r="D300" s="9"/>
       <c r="F300" s="9"/>
@@ -6392,7 +6382,7 @@
       <c r="K300" s="9"/>
       <c r="L300" s="9"/>
     </row>
-    <row r="301" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C301" s="9"/>
       <c r="D301" s="9"/>
       <c r="F301" s="9"/>
@@ -6403,7 +6393,7 @@
       <c r="K301" s="9"/>
       <c r="L301" s="9"/>
     </row>
-    <row r="302" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C302" s="9"/>
       <c r="D302" s="9"/>
       <c r="F302" s="9"/>
@@ -6414,7 +6404,7 @@
       <c r="K302" s="9"/>
       <c r="L302" s="9"/>
     </row>
-    <row r="303" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C303" s="9"/>
       <c r="D303" s="9"/>
       <c r="F303" s="9"/>
@@ -6425,7 +6415,7 @@
       <c r="K303" s="9"/>
       <c r="L303" s="9"/>
     </row>
-    <row r="304" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C304" s="9"/>
       <c r="D304" s="9"/>
       <c r="F304" s="9"/>
@@ -6436,7 +6426,7 @@
       <c r="K304" s="9"/>
       <c r="L304" s="9"/>
     </row>
-    <row r="305" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C305" s="9"/>
       <c r="D305" s="9"/>
       <c r="F305" s="9"/>
@@ -6447,7 +6437,7 @@
       <c r="K305" s="9"/>
       <c r="L305" s="9"/>
     </row>
-    <row r="306" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C306" s="9"/>
       <c r="D306" s="9"/>
       <c r="F306" s="9"/>
@@ -6458,7 +6448,7 @@
       <c r="K306" s="9"/>
       <c r="L306" s="9"/>
     </row>
-    <row r="307" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C307" s="9"/>
       <c r="D307" s="9"/>
       <c r="F307" s="9"/>
@@ -6469,7 +6459,7 @@
       <c r="K307" s="9"/>
       <c r="L307" s="9"/>
     </row>
-    <row r="308" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C308" s="9"/>
       <c r="D308" s="9"/>
       <c r="F308" s="9"/>
@@ -6480,7 +6470,7 @@
       <c r="K308" s="9"/>
       <c r="L308" s="9"/>
     </row>
-    <row r="309" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C309" s="9"/>
       <c r="D309" s="9"/>
       <c r="F309" s="9"/>
@@ -6491,7 +6481,7 @@
       <c r="K309" s="9"/>
       <c r="L309" s="9"/>
     </row>
-    <row r="310" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C310" s="9"/>
       <c r="D310" s="9"/>
       <c r="F310" s="9"/>
@@ -6502,7 +6492,7 @@
       <c r="K310" s="9"/>
       <c r="L310" s="9"/>
     </row>
-    <row r="311" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C311" s="9"/>
       <c r="D311" s="9"/>
       <c r="F311" s="9"/>
@@ -6513,7 +6503,7 @@
       <c r="K311" s="9"/>
       <c r="L311" s="9"/>
     </row>
-    <row r="312" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C312" s="9"/>
       <c r="D312" s="9"/>
       <c r="F312" s="9"/>
@@ -6524,7 +6514,7 @@
       <c r="K312" s="9"/>
       <c r="L312" s="9"/>
     </row>
-    <row r="313" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C313" s="9"/>
       <c r="D313" s="9"/>
       <c r="F313" s="9"/>
@@ -6535,7 +6525,7 @@
       <c r="K313" s="9"/>
       <c r="L313" s="9"/>
     </row>
-    <row r="314" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C314" s="9"/>
       <c r="D314" s="9"/>
       <c r="F314" s="9"/>
@@ -6546,7 +6536,7 @@
       <c r="K314" s="9"/>
       <c r="L314" s="9"/>
     </row>
-    <row r="315" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C315" s="9"/>
       <c r="D315" s="9"/>
       <c r="F315" s="9"/>
@@ -6557,7 +6547,7 @@
       <c r="K315" s="9"/>
       <c r="L315" s="9"/>
     </row>
-    <row r="316" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C316" s="9"/>
       <c r="D316" s="9"/>
       <c r="F316" s="9"/>
@@ -6568,7 +6558,7 @@
       <c r="K316" s="9"/>
       <c r="L316" s="9"/>
     </row>
-    <row r="317" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C317" s="9"/>
       <c r="D317" s="9"/>
       <c r="F317" s="9"/>
@@ -6579,7 +6569,7 @@
       <c r="K317" s="9"/>
       <c r="L317" s="9"/>
     </row>
-    <row r="318" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C318" s="9"/>
       <c r="D318" s="9"/>
       <c r="F318" s="9"/>
@@ -6590,7 +6580,7 @@
       <c r="K318" s="9"/>
       <c r="L318" s="9"/>
     </row>
-    <row r="319" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C319" s="9"/>
       <c r="D319" s="9"/>
       <c r="F319" s="9"/>
@@ -6601,7 +6591,7 @@
       <c r="K319" s="9"/>
       <c r="L319" s="9"/>
     </row>
-    <row r="320" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C320" s="9"/>
       <c r="D320" s="9"/>
       <c r="F320" s="9"/>
@@ -6612,7 +6602,7 @@
       <c r="K320" s="9"/>
       <c r="L320" s="9"/>
     </row>
-    <row r="321" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C321" s="9"/>
       <c r="D321" s="9"/>
       <c r="F321" s="9"/>
@@ -6623,7 +6613,7 @@
       <c r="K321" s="9"/>
       <c r="L321" s="9"/>
     </row>
-    <row r="322" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C322" s="9"/>
       <c r="D322" s="9"/>
       <c r="F322" s="9"/>
@@ -6634,7 +6624,7 @@
       <c r="K322" s="9"/>
       <c r="L322" s="9"/>
     </row>
-    <row r="323" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C323" s="9"/>
       <c r="D323" s="9"/>
       <c r="F323" s="9"/>
@@ -6645,7 +6635,7 @@
       <c r="K323" s="9"/>
       <c r="L323" s="9"/>
     </row>
-    <row r="324" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C324" s="9"/>
       <c r="D324" s="9"/>
       <c r="F324" s="9"/>
@@ -6656,7 +6646,7 @@
       <c r="K324" s="9"/>
       <c r="L324" s="9"/>
     </row>
-    <row r="325" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C325" s="9"/>
       <c r="D325" s="9"/>
       <c r="F325" s="9"/>
@@ -6667,7 +6657,7 @@
       <c r="K325" s="9"/>
       <c r="L325" s="9"/>
     </row>
-    <row r="326" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C326" s="9"/>
       <c r="D326" s="9"/>
       <c r="F326" s="9"/>
@@ -6678,7 +6668,7 @@
       <c r="K326" s="9"/>
       <c r="L326" s="9"/>
     </row>
-    <row r="327" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C327" s="9"/>
       <c r="D327" s="9"/>
       <c r="F327" s="9"/>
@@ -6689,7 +6679,7 @@
       <c r="K327" s="9"/>
       <c r="L327" s="9"/>
     </row>
-    <row r="328" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C328" s="9"/>
       <c r="D328" s="9"/>
       <c r="F328" s="9"/>
@@ -6700,7 +6690,7 @@
       <c r="K328" s="9"/>
       <c r="L328" s="9"/>
     </row>
-    <row r="329" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C329" s="9"/>
       <c r="D329" s="9"/>
       <c r="F329" s="9"/>
@@ -6711,7 +6701,7 @@
       <c r="K329" s="9"/>
       <c r="L329" s="9"/>
     </row>
-    <row r="330" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C330" s="9"/>
       <c r="D330" s="9"/>
       <c r="F330" s="9"/>
@@ -6722,7 +6712,7 @@
       <c r="K330" s="9"/>
       <c r="L330" s="9"/>
     </row>
-    <row r="331" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C331" s="9"/>
       <c r="D331" s="9"/>
       <c r="F331" s="9"/>
@@ -6733,7 +6723,7 @@
       <c r="K331" s="9"/>
       <c r="L331" s="9"/>
     </row>
-    <row r="332" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C332" s="9"/>
       <c r="D332" s="9"/>
       <c r="F332" s="9"/>
@@ -6744,7 +6734,7 @@
       <c r="K332" s="9"/>
       <c r="L332" s="9"/>
     </row>
-    <row r="333" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C333" s="9"/>
       <c r="D333" s="9"/>
       <c r="F333" s="9"/>
@@ -6755,7 +6745,7 @@
       <c r="K333" s="9"/>
       <c r="L333" s="9"/>
     </row>
-    <row r="334" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C334" s="9"/>
       <c r="D334" s="9"/>
       <c r="F334" s="9"/>
@@ -6766,7 +6756,7 @@
       <c r="K334" s="9"/>
       <c r="L334" s="9"/>
     </row>
-    <row r="335" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C335" s="9"/>
       <c r="D335" s="9"/>
       <c r="F335" s="9"/>
@@ -6777,7 +6767,7 @@
       <c r="K335" s="9"/>
       <c r="L335" s="9"/>
     </row>
-    <row r="336" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C336" s="9"/>
       <c r="D336" s="9"/>
       <c r="F336" s="9"/>
@@ -6788,7 +6778,7 @@
       <c r="K336" s="9"/>
       <c r="L336" s="9"/>
     </row>
-    <row r="337" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C337" s="9"/>
       <c r="D337" s="9"/>
       <c r="F337" s="9"/>
@@ -6799,7 +6789,7 @@
       <c r="K337" s="9"/>
       <c r="L337" s="9"/>
     </row>
-    <row r="338" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C338" s="9"/>
       <c r="D338" s="9"/>
       <c r="F338" s="9"/>
@@ -6810,7 +6800,7 @@
       <c r="K338" s="9"/>
       <c r="L338" s="9"/>
     </row>
-    <row r="339" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C339" s="9"/>
       <c r="D339" s="9"/>
       <c r="F339" s="9"/>
@@ -6821,7 +6811,7 @@
       <c r="K339" s="9"/>
       <c r="L339" s="9"/>
     </row>
-    <row r="340" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C340" s="9"/>
       <c r="D340" s="9"/>
       <c r="F340" s="9"/>
@@ -6832,7 +6822,7 @@
       <c r="K340" s="9"/>
       <c r="L340" s="9"/>
     </row>
-    <row r="341" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C341" s="9"/>
       <c r="D341" s="9"/>
       <c r="F341" s="9"/>
@@ -6843,7 +6833,7 @@
       <c r="K341" s="9"/>
       <c r="L341" s="9"/>
     </row>
-    <row r="342" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C342" s="9"/>
       <c r="D342" s="9"/>
       <c r="F342" s="9"/>
@@ -6854,7 +6844,7 @@
       <c r="K342" s="9"/>
       <c r="L342" s="9"/>
     </row>
-    <row r="343" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C343" s="9"/>
       <c r="D343" s="9"/>
       <c r="F343" s="9"/>
@@ -6865,7 +6855,7 @@
       <c r="K343" s="9"/>
       <c r="L343" s="9"/>
     </row>
-    <row r="344" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C344" s="9"/>
       <c r="D344" s="9"/>
       <c r="F344" s="9"/>
@@ -6876,7 +6866,7 @@
       <c r="K344" s="9"/>
       <c r="L344" s="9"/>
     </row>
-    <row r="345" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C345" s="9"/>
       <c r="D345" s="9"/>
       <c r="F345" s="9"/>
@@ -6887,7 +6877,7 @@
       <c r="K345" s="9"/>
       <c r="L345" s="9"/>
     </row>
-    <row r="346" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C346" s="9"/>
       <c r="D346" s="9"/>
       <c r="F346" s="9"/>
@@ -6898,7 +6888,7 @@
       <c r="K346" s="9"/>
       <c r="L346" s="9"/>
     </row>
-    <row r="347" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C347" s="9"/>
       <c r="D347" s="9"/>
       <c r="F347" s="9"/>
@@ -6909,7 +6899,7 @@
       <c r="K347" s="9"/>
       <c r="L347" s="9"/>
     </row>
-    <row r="348" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C348" s="9"/>
       <c r="D348" s="9"/>
       <c r="F348" s="9"/>
@@ -6920,7 +6910,7 @@
       <c r="K348" s="9"/>
       <c r="L348" s="9"/>
     </row>
-    <row r="349" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C349" s="9"/>
       <c r="D349" s="9"/>
       <c r="F349" s="9"/>
@@ -6931,7 +6921,7 @@
       <c r="K349" s="9"/>
       <c r="L349" s="9"/>
     </row>
-    <row r="350" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C350" s="9"/>
       <c r="D350" s="9"/>
       <c r="F350" s="9"/>
@@ -6942,7 +6932,7 @@
       <c r="K350" s="9"/>
       <c r="L350" s="9"/>
     </row>
-    <row r="351" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C351" s="9"/>
       <c r="D351" s="9"/>
       <c r="F351" s="9"/>
@@ -6953,7 +6943,7 @@
       <c r="K351" s="9"/>
       <c r="L351" s="9"/>
     </row>
-    <row r="352" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C352" s="9"/>
       <c r="D352" s="9"/>
       <c r="F352" s="9"/>
@@ -6964,7 +6954,7 @@
       <c r="K352" s="9"/>
       <c r="L352" s="9"/>
     </row>
-    <row r="353" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C353" s="9"/>
       <c r="D353" s="9"/>
       <c r="F353" s="9"/>
@@ -6975,7 +6965,7 @@
       <c r="K353" s="9"/>
       <c r="L353" s="9"/>
     </row>
-    <row r="354" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C354" s="9"/>
       <c r="D354" s="9"/>
       <c r="F354" s="9"/>
@@ -6986,7 +6976,7 @@
       <c r="K354" s="9"/>
       <c r="L354" s="9"/>
     </row>
-    <row r="355" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C355" s="9"/>
       <c r="D355" s="9"/>
       <c r="F355" s="9"/>
@@ -6997,7 +6987,7 @@
       <c r="K355" s="9"/>
       <c r="L355" s="9"/>
     </row>
-    <row r="356" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C356" s="9"/>
       <c r="D356" s="9"/>
       <c r="F356" s="9"/>
@@ -7008,7 +6998,7 @@
       <c r="K356" s="9"/>
       <c r="L356" s="9"/>
     </row>
-    <row r="357" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C357" s="9"/>
       <c r="D357" s="9"/>
       <c r="F357" s="9"/>
@@ -7019,7 +7009,7 @@
       <c r="K357" s="9"/>
       <c r="L357" s="9"/>
     </row>
-    <row r="358" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C358" s="9"/>
       <c r="D358" s="9"/>
       <c r="F358" s="9"/>
@@ -7030,7 +7020,7 @@
       <c r="K358" s="9"/>
       <c r="L358" s="9"/>
     </row>
-    <row r="359" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C359" s="9"/>
       <c r="D359" s="9"/>
       <c r="F359" s="9"/>
@@ -7041,7 +7031,7 @@
       <c r="K359" s="9"/>
       <c r="L359" s="9"/>
     </row>
-    <row r="360" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C360" s="9"/>
       <c r="D360" s="9"/>
       <c r="F360" s="9"/>
@@ -7052,7 +7042,7 @@
       <c r="K360" s="9"/>
       <c r="L360" s="9"/>
     </row>
-    <row r="361" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C361" s="9"/>
       <c r="D361" s="9"/>
       <c r="F361" s="9"/>
@@ -7063,7 +7053,7 @@
       <c r="K361" s="9"/>
       <c r="L361" s="9"/>
     </row>
-    <row r="362" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C362" s="9"/>
       <c r="D362" s="9"/>
       <c r="F362" s="9"/>
@@ -7074,7 +7064,7 @@
       <c r="K362" s="9"/>
       <c r="L362" s="9"/>
     </row>
-    <row r="363" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C363" s="9"/>
       <c r="D363" s="9"/>
       <c r="F363" s="9"/>
@@ -7085,7 +7075,7 @@
       <c r="K363" s="9"/>
       <c r="L363" s="9"/>
     </row>
-    <row r="364" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C364" s="9"/>
       <c r="D364" s="9"/>
       <c r="F364" s="9"/>
@@ -7096,7 +7086,7 @@
       <c r="K364" s="9"/>
       <c r="L364" s="9"/>
     </row>
-    <row r="365" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C365" s="9"/>
       <c r="D365" s="9"/>
       <c r="F365" s="9"/>
@@ -7107,7 +7097,7 @@
       <c r="K365" s="9"/>
       <c r="L365" s="9"/>
     </row>
-    <row r="366" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C366" s="9"/>
       <c r="D366" s="9"/>
       <c r="F366" s="9"/>
@@ -7118,7 +7108,7 @@
       <c r="K366" s="9"/>
       <c r="L366" s="9"/>
     </row>
-    <row r="367" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C367" s="9"/>
       <c r="D367" s="9"/>
       <c r="F367" s="9"/>
@@ -7129,7 +7119,7 @@
       <c r="K367" s="9"/>
       <c r="L367" s="9"/>
     </row>
-    <row r="368" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C368" s="9"/>
       <c r="D368" s="9"/>
       <c r="F368" s="9"/>
@@ -7140,7 +7130,7 @@
       <c r="K368" s="9"/>
       <c r="L368" s="9"/>
     </row>
-    <row r="369" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C369" s="9"/>
       <c r="D369" s="9"/>
       <c r="F369" s="9"/>
@@ -7151,7 +7141,7 @@
       <c r="K369" s="9"/>
       <c r="L369" s="9"/>
     </row>
-    <row r="370" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C370" s="9"/>
       <c r="D370" s="9"/>
       <c r="F370" s="9"/>
@@ -7162,7 +7152,7 @@
       <c r="K370" s="9"/>
       <c r="L370" s="9"/>
     </row>
-    <row r="371" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C371" s="9"/>
       <c r="D371" s="9"/>
       <c r="F371" s="9"/>
@@ -7173,7 +7163,7 @@
       <c r="K371" s="9"/>
       <c r="L371" s="9"/>
     </row>
-    <row r="372" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C372" s="9"/>
       <c r="D372" s="9"/>
       <c r="F372" s="9"/>
@@ -7184,7 +7174,7 @@
       <c r="K372" s="9"/>
       <c r="L372" s="9"/>
     </row>
-    <row r="373" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C373" s="9"/>
       <c r="D373" s="9"/>
       <c r="F373" s="9"/>
@@ -7195,7 +7185,7 @@
       <c r="K373" s="9"/>
       <c r="L373" s="9"/>
     </row>
-    <row r="374" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C374" s="9"/>
       <c r="D374" s="9"/>
       <c r="F374" s="9"/>

</xml_diff>

<commit_message>
stuff a lot of stuff
</commit_message>
<xml_diff>
--- a/docs/Comparison.xlsx
+++ b/docs/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\xcom2_my_tweaks\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAC2711-B60F-468B-9710-DD09C2E93EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B05092E-57AB-41E1-8D75-BDD74DE9B944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6D18C04-5EFF-4A90-9265-84C7107E118D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="385">
   <si>
     <t>Comparison</t>
   </si>
@@ -697,9 +697,6 @@
     <t>BScav</t>
   </si>
   <si>
-    <t>Bullpup_CV</t>
-  </si>
-  <si>
     <t>WOTC_APA_TacticalFlexibility (IRI_ResupplyAmmo, ARFMLootCorpse, IRI_BandageThrow)</t>
   </si>
   <si>
@@ -808,9 +805,6 @@
     <t>Tank</t>
   </si>
   <si>
-    <t>Hunter(P)</t>
-  </si>
-  <si>
     <t>Hunty</t>
   </si>
   <si>
@@ -832,9 +826,6 @@
     <t>IRI_BH_NamedBullet</t>
   </si>
   <si>
-    <t>Dualist(S)</t>
-  </si>
-  <si>
     <t>BGunslinger</t>
   </si>
   <si>
@@ -886,15 +877,9 @@
     <t>BRocky</t>
   </si>
   <si>
-    <t>Marauder(S)</t>
-  </si>
-  <si>
     <t>BMarauder</t>
   </si>
   <si>
-    <t>WOTC_APA_Marauder</t>
-  </si>
-  <si>
     <t>WOTC_APA_FlushEmOut</t>
   </si>
   <si>
@@ -904,9 +889,6 @@
     <t>WOTC_APA_ExplosiveAction</t>
   </si>
   <si>
-    <t>WOTC_APA_CloseCombatSpecialist</t>
-  </si>
-  <si>
     <t>LW2WotC_HitandRun</t>
   </si>
   <si>
@@ -1019,9 +1001,6 @@
   </si>
   <si>
     <t>(ShadowOps_StealthProtocol or MZCombatScanner or WOTC_APA_UpgradedScanners)</t>
-  </si>
-  <si>
-    <t>WOTC_APA_Harass (IRI_BH_Headhunter, IRI_BH_Nightfall_Passive, IRI_BH_Nightfall)</t>
   </si>
   <si>
     <t>Gremlin_CV (IntrusionProtocol, WOTC_APA_Failsafe)</t>
@@ -1213,9 +1192,6 @@
     <t>Sword_CV</t>
   </si>
   <si>
-    <t>Enforcer(T)</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -1223,13 +1199,94 @@
   </si>
   <si>
     <t>SMG_CV (StrafingShot, Spray)</t>
+  </si>
+  <si>
+    <t>Hunter(S)</t>
+  </si>
+  <si>
+    <t>IRI_BH_Headhunter (IRI_BH_Nightfall_Passive, IRI_BH_Nightfall)</t>
+  </si>
+  <si>
+    <t>Marauder(P)</t>
+  </si>
+  <si>
+    <t>Bullpup_CV (WOTC_APA_Marauder)</t>
+  </si>
+  <si>
+    <t>Dualist(T)</t>
+  </si>
+  <si>
+    <t>WOTC_APA_Harass (WOTC_APA_Skirmisher)</t>
+  </si>
+  <si>
+    <t>INHIBITING_SHOT</t>
+  </si>
+  <si>
+    <t>Electrician(T)</t>
+  </si>
+  <si>
+    <t>Gunner(P)</t>
+  </si>
+  <si>
+    <t>WOTC_APA_FireDiscipline (WOTC_APA_SustainedFire, LW2WotC_AreaSuppression)</t>
+  </si>
+  <si>
+    <t>F_Havoc</t>
+  </si>
+  <si>
+    <t>AGunner</t>
+  </si>
+  <si>
+    <t>F_SuppressingFire</t>
+  </si>
+  <si>
+    <t>F_ControlledFire</t>
+  </si>
+  <si>
+    <t>LW2WotC_DangerZone</t>
+  </si>
+  <si>
+    <t>F_ThousandsToGo</t>
+  </si>
+  <si>
+    <t>MZPanicSuppression</t>
+  </si>
+  <si>
+    <t>F_KillEmAll</t>
+  </si>
+  <si>
+    <t>Infantry(P)</t>
+  </si>
+  <si>
+    <t>AInfantry</t>
+  </si>
+  <si>
+    <t>CoveringFire</t>
+  </si>
+  <si>
+    <t>WOTC_APA_PinEmDown</t>
+  </si>
+  <si>
+    <t>WOTC_APA_Emplaced</t>
+  </si>
+  <si>
+    <t>WOTC_APA_LightEmUp</t>
+  </si>
+  <si>
+    <t>WOTC_APA_TacticalSense</t>
+  </si>
+  <si>
+    <t>F_FireFirst</t>
+  </si>
+  <si>
+    <t>Cannon (Suppression, LW2WotC_CyclicFire)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1290,8 +1347,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1388,6 +1452,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1401,7 +1471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1513,6 +1583,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1854,10 +1930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A043E2-6980-4E69-B156-F69EB3A846AD}">
-  <dimension ref="A1:M375"/>
+  <dimension ref="A1:M379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,7 +1988,7 @@
     <row r="3" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="37"/>
@@ -1965,13 +2041,13 @@
     </row>
     <row r="5" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -1996,37 +2072,37 @@
     </row>
     <row r="7" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F7" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2044,37 +2120,37 @@
     </row>
     <row r="9" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>231</v>
-      </c>
       <c r="L9" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2092,13 +2168,13 @@
     </row>
     <row r="11" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -2123,13 +2199,13 @@
     </row>
     <row r="13" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -2259,7 +2335,7 @@
         <v>83</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>84</v>
@@ -2304,37 +2380,37 @@
     </row>
     <row r="21" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E21" s="14" t="s">
+      <c r="K21" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2353,7 +2429,7 @@
     <row r="23" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="36" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C23" s="36"/>
       <c r="D23" s="37"/>
@@ -2415,7 +2491,7 @@
         <v>159</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>168</v>
@@ -2460,7 +2536,7 @@
         <v>176</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>177</v>
@@ -2502,22 +2578,22 @@
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>158</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F29" s="27" t="s">
         <v>160</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>161</v>
@@ -2550,7 +2626,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>192</v>
@@ -2599,7 +2675,7 @@
     <row r="33" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="36" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C33" s="36"/>
       <c r="D33" s="37"/>
@@ -2652,37 +2728,37 @@
     </row>
     <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>309</v>
+        <v>369</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>384</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>124</v>
+        <v>368</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>125</v>
+        <v>370</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>126</v>
+        <v>371</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>127</v>
+        <v>372</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>128</v>
+        <v>373</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>130</v>
+        <v>374</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>129</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2698,39 +2774,39 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>35</v>
+        <v>376</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>157</v>
+        <v>377</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>12</v>
+        <v>303</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>36</v>
+        <v>367</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>30</v>
+        <v>378</v>
+      </c>
+      <c r="G37" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>33</v>
+        <v>380</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>38</v>
+        <v>381</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>34</v>
+        <v>382</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>39</v>
+        <v>383</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2746,39 +2822,39 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>312</v>
+        <v>122</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>313</v>
+        <v>123</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>12</v>
+        <v>303</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>110</v>
+        <v>124</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>316</v>
+        <v>127</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>317</v>
+        <v>130</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>318</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2794,93 +2870,87 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="8"/>
-    </row>
-    <row r="42" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" s="8"/>
-    </row>
-    <row r="43" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>64</v>
+    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>306</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>360</v>
+        <v>307</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>359</v>
+        <v>12</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>308</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G43" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="H43" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J43" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="L43" s="3" t="s">
-        <v>70</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2896,87 +2966,93 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-    </row>
-    <row r="47" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
-        <v>249</v>
+    <row r="45" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" s="8"/>
+    </row>
+    <row r="47" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>250</v>
+        <v>353</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>320</v>
+        <v>65</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>352</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>252</v>
+        <v>66</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>253</v>
+        <v>305</v>
+      </c>
+      <c r="H47" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>254</v>
+        <v>67</v>
+      </c>
+      <c r="J47" s="32" t="s">
+        <v>68</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>255</v>
+        <v>69</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>256</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2992,42 +3068,42 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>294</v>
+        <v>112</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>295</v>
+        <v>113</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>351</v>
+        <v>115</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>352</v>
+        <v>114</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>353</v>
+        <v>116</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>354</v>
+        <v>117</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>356</v>
+        <v>13</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>358</v>
+        <v>118</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>357</v>
+        <v>119</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>355</v>
+        <v>120</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -3040,25 +3116,42 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="38" t="s">
+        <v>360</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="E51" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="J51" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="K51" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -3071,25 +3164,42 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="11" t="s">
-        <v>259</v>
+    <row r="53" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -3102,42 +3212,25 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="J55" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -3150,25 +3243,42 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
-        <v>300</v>
+    <row r="57" spans="2:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="38" t="s">
+        <v>358</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>301</v>
+        <v>248</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -3181,32 +3291,25 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
-        <v>362</v>
+        <v>294</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>205</v>
+        <v>295</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -3219,96 +3322,63 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="B61" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="8"/>
-    </row>
-    <row r="62" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
-      <c r="B62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L62" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M62" s="8"/>
-    </row>
-    <row r="63" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+    </row>
+    <row r="63" spans="2:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="s">
-        <v>11</v>
+        <v>365</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>307</v>
+        <v>355</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I63" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
       <c r="L63" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -3321,87 +3391,93 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I65" s="16" t="s">
+    <row r="65" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="26"/>
+      <c r="B65" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="8"/>
+    </row>
+    <row r="66" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="26"/>
+      <c r="B66" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M66" s="8"/>
+    </row>
+    <row r="67" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J65" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="K65" s="3" t="s">
+      <c r="J67" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K67" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L65" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-    </row>
-    <row r="67" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B67" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I67" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="L67" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3417,93 +3493,87 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="26"/>
-      <c r="B69" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C69" s="36"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="8"/>
-    </row>
-    <row r="70" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
-      <c r="B70" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E70" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L70" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M70" s="8"/>
-    </row>
-    <row r="71" spans="1:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
-        <v>43</v>
+    <row r="69" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I69" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B71" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3519,87 +3589,93 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-    </row>
-    <row r="75" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="26"/>
+      <c r="B73" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="36"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="8"/>
+    </row>
+    <row r="74" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="26"/>
+      <c r="B74" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M74" s="8"/>
+    </row>
+    <row r="75" spans="1:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="11" t="s">
-        <v>306</v>
+        <v>43</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>212</v>
+        <v>45</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>213</v>
+        <v>46</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>214</v>
+        <v>47</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>215</v>
+        <v>48</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>216</v>
+        <v>49</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>217</v>
+        <v>49</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>218</v>
+        <v>50</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>219</v>
+        <v>51</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>220</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -3615,39 +3691,39 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="11" t="s">
-        <v>241</v>
+        <v>72</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>242</v>
+        <v>73</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>243</v>
+        <v>75</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>244</v>
+        <v>76</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>244</v>
+        <v>77</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>245</v>
+        <v>78</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>245</v>
+        <v>79</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>246</v>
+        <v>80</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>246</v>
+        <v>81</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>247</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -3663,39 +3739,39 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="11" t="s">
-        <v>262</v>
+        <v>300</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>74</v>
+        <v>211</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>361</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>264</v>
+        <v>212</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>266</v>
+        <v>215</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -3711,23 +3787,40 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="s">
-        <v>305</v>
+        <v>240</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>302</v>
+        <v>241</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
+        <v>24</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B82" s="5"/>
@@ -3744,21 +3837,38 @@
     </row>
     <row r="83" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="11" t="s">
-        <v>298</v>
+        <v>259</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>299</v>
+        <v>260</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="15"/>
+        <v>74</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="L83" s="3" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
@@ -3773,94 +3883,54 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
-      <c r="B85" s="36" t="s">
-        <v>330</v>
-      </c>
-      <c r="C85" s="36"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="8"/>
-    </row>
-    <row r="86" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
-      <c r="B86" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H86" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I86" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L86" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M86" s="8"/>
-    </row>
-    <row r="87" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="3" t="s">
-        <v>40</v>
+    <row r="85" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+    </row>
+    <row r="87" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="11" t="s">
+        <v>292</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>41</v>
+        <v>293</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="L87" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
@@ -3875,87 +3945,93 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B89" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C89" s="3" t="s">
+    <row r="89" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="26"/>
+      <c r="B89" s="36" t="s">
         <v>323</v>
       </c>
-      <c r="D89" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="I89" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J89" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="L89" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5"/>
-      <c r="K90" s="5"/>
-      <c r="L90" s="5"/>
-    </row>
-    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="C89" s="36"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="8"/>
+    </row>
+    <row r="90" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="26"/>
+      <c r="B90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M90" s="8"/>
+    </row>
+    <row r="91" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>131</v>
+        <v>41</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>136</v>
+        <v>321</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>137</v>
+        <v>313</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>138</v>
+        <v>313</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>139</v>
+        <v>313</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>141</v>
+        <v>340</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K91" s="9" t="s">
-        <v>142</v>
+        <v>340</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>340</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>332</v>
+        <v>42</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -3973,37 +4049,37 @@
     </row>
     <row r="93" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>145</v>
+        <v>315</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="E93" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="F93" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="G93" s="35" t="s">
-        <v>25</v>
+        <v>316</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>318</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>27</v>
+        <v>319</v>
       </c>
       <c r="I93" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J93" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K93" s="31" t="s">
-        <v>68</v>
+      <c r="J93" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4016,42 +4092,42 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
-      <c r="K94" s="10"/>
+      <c r="K94" s="5"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>333</v>
+        <v>135</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>12</v>
+        <v>143</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>334</v>
+        <v>136</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>340</v>
+        <v>138</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>341</v>
+        <v>139</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>337</v>
+        <v>141</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>336</v>
+        <v>140</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>342</v>
+        <v>142</v>
       </c>
       <c r="L95" s="3" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4064,96 +4140,90 @@
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
-      <c r="K96" s="10"/>
+      <c r="K96" s="5"/>
       <c r="L96" s="5"/>
     </row>
-    <row r="97" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
-      <c r="B97" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="C97" s="36"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
-      <c r="M97" s="8"/>
-    </row>
-    <row r="98" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
-      <c r="B98" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G98" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H98" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I98" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K98" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L98" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M98" s="8"/>
-    </row>
-    <row r="99" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="13" t="s">
-        <v>193</v>
+    <row r="97" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B97" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="E97" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="F97" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="G97" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K97" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="L97" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="5"/>
+    </row>
+    <row r="99" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
+        <v>326</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>194</v>
+        <v>328</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E99" s="14" t="s">
-        <v>196</v>
+        <v>12</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>197</v>
+        <v>332</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>198</v>
+        <v>333</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>199</v>
+        <v>334</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>200</v>
+        <v>330</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>202</v>
+        <v>329</v>
+      </c>
+      <c r="K99" s="9" t="s">
+        <v>335</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>203</v>
+        <v>336</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4166,227 +4236,233 @@
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
+      <c r="K100" s="10"/>
       <c r="L100" s="5"/>
     </row>
-    <row r="101" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B101" s="11" t="s">
+    <row r="101" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="26"/>
+      <c r="B101" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="C101" s="36"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="8"/>
+    </row>
+    <row r="102" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="26"/>
+      <c r="B102" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L102" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M102" s="8"/>
+    </row>
+    <row r="103" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E103" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5"/>
+    </row>
+    <row r="105" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B105" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E101" s="14" t="s">
+      <c r="E105" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="F105" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G101" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H101" s="3" t="s">
+      <c r="H105" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I101" s="3" t="s">
+      <c r="I105" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J101" s="3" t="s">
+      <c r="J105" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="K101" s="3" t="s">
+      <c r="K105" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="L101" s="3" t="s">
+      <c r="L105" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
-      <c r="B102" s="36" t="s">
+    <row r="106" spans="1:13" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="26"/>
+      <c r="B106" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C102" s="36"/>
-      <c r="D102" s="37"/>
-      <c r="E102" s="21"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="8"/>
-    </row>
-    <row r="103" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
-      <c r="B103" s="12" t="s">
+      <c r="C106" s="36"/>
+      <c r="D106" s="37"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+      <c r="M106" s="8"/>
+    </row>
+    <row r="107" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="26"/>
+      <c r="B107" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E103" s="22" t="s">
+      <c r="E107" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F103" s="4" t="s">
+      <c r="F107" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G103" s="4" t="s">
+      <c r="G107" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H103" s="4" t="s">
+      <c r="H107" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I103" s="4" t="s">
+      <c r="I107" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J103" s="4" t="s">
+      <c r="J107" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K103" s="4" t="s">
+      <c r="K107" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L103" s="4" t="s">
+      <c r="L107" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M103" s="8"/>
-    </row>
-    <row r="104" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B104" s="11" t="s">
+      <c r="M107" s="8"/>
+    </row>
+    <row r="108" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B108" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E104" s="14" t="s">
+      <c r="E108" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F104" s="3" t="s">
+      <c r="F108" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G104" s="3" t="s">
+      <c r="G108" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H104" s="3" t="s">
+      <c r="H108" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I104" s="3" t="s">
+      <c r="I108" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J104" s="3" t="s">
+      <c r="J108" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="K104" s="3" t="s">
+      <c r="K108" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="L104" s="3" t="s">
+      <c r="L108" s="3" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
-      <c r="L105" s="5"/>
-    </row>
-    <row r="106" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E106" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H106" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K106" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L106" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-      <c r="K107" s="5"/>
-      <c r="L107" s="5"/>
-    </row>
-    <row r="108" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="E108" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H108" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J108" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K108" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L108" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4402,23 +4478,40 @@
       <c r="K109" s="5"/>
       <c r="L109" s="5"/>
     </row>
-    <row r="110" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="11" t="s">
-        <v>296</v>
+        <v>103</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>297</v>
+        <v>104</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F110" s="15"/>
-      <c r="G110" s="15"/>
-      <c r="H110" s="15"/>
-      <c r="I110" s="15"/>
-      <c r="J110" s="15"/>
-      <c r="K110" s="15"/>
-      <c r="L110" s="15"/>
+        <v>314</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B111" s="5"/>
@@ -4433,219 +4526,162 @@
       <c r="K111" s="5"/>
       <c r="L111" s="5"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A112" s="17"/>
-      <c r="B112" s="3"/>
-      <c r="E112" s="3"/>
-      <c r="M112" s="17"/>
-    </row>
-    <row r="113" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="3"/>
-    </row>
-    <row r="114" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
-      <c r="H114" s="3"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-      <c r="L114" s="3"/>
-    </row>
-    <row r="115" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
-      <c r="H115" s="3"/>
-      <c r="I115" s="3"/>
-      <c r="J115" s="3"/>
-      <c r="K115" s="3"/>
-      <c r="L115" s="3"/>
-    </row>
-    <row r="116" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L112" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+      <c r="I113" s="5"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+      <c r="L113" s="5"/>
+    </row>
+    <row r="114" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
+      <c r="H114" s="15"/>
+      <c r="I114" s="15"/>
+      <c r="J114" s="15"/>
+      <c r="K114" s="15"/>
+      <c r="L114" s="15"/>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" s="17"/>
       <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="3"/>
-      <c r="H116" s="3"/>
-      <c r="I116" s="3"/>
-      <c r="J116" s="3"/>
-      <c r="K116" s="3"/>
-      <c r="L116" s="3"/>
-    </row>
-    <row r="117" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M116" s="17"/>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117" s="17"/>
       <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-      <c r="J117" s="3"/>
-      <c r="K117" s="3"/>
-      <c r="L117" s="3"/>
-    </row>
-    <row r="118" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M117" s="17"/>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118" s="17"/>
       <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
-      <c r="L118" s="3"/>
-    </row>
-    <row r="119" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M118" s="17"/>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" s="17"/>
       <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
-      <c r="J119" s="3"/>
-      <c r="K119" s="3"/>
-      <c r="L119" s="3"/>
-    </row>
-    <row r="120" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M119" s="17"/>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120" s="17"/>
       <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="3"/>
-      <c r="L120" s="3"/>
-    </row>
-    <row r="121" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M120" s="17"/>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121" s="17"/>
       <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3"/>
-      <c r="J121" s="3"/>
-      <c r="K121" s="3"/>
-      <c r="L121" s="3"/>
-    </row>
-    <row r="122" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M121" s="17"/>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" s="17"/>
       <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
-    </row>
-    <row r="123" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M122" s="17"/>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123" s="17"/>
       <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="3"/>
-      <c r="K123" s="3"/>
-      <c r="L123" s="3"/>
-    </row>
-    <row r="124" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M123" s="17"/>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124" s="17"/>
       <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
       <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
-      <c r="L124" s="3"/>
-    </row>
-    <row r="125" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M124" s="17"/>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125" s="17"/>
       <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="3"/>
-      <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
-      <c r="J125" s="3"/>
-      <c r="K125" s="3"/>
-      <c r="L125" s="3"/>
-    </row>
-    <row r="126" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M125" s="17"/>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126" s="17"/>
       <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
-      <c r="H126" s="3"/>
-      <c r="I126" s="3"/>
-      <c r="J126" s="3"/>
-      <c r="K126" s="3"/>
-      <c r="L126" s="3"/>
-    </row>
-    <row r="127" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M126" s="17"/>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127" s="17"/>
       <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="3"/>
-      <c r="H127" s="3"/>
-      <c r="I127" s="3"/>
-      <c r="J127" s="3"/>
-      <c r="K127" s="3"/>
-      <c r="L127" s="3"/>
-    </row>
-    <row r="128" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M127" s="17"/>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128" s="17"/>
       <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="3"/>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="3"/>
-      <c r="K128" s="3"/>
-      <c r="L128" s="3"/>
+      <c r="M128" s="17"/>
     </row>
     <row r="129" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="3"/>
@@ -7767,58 +7803,159 @@
       <c r="K368" s="3"/>
       <c r="L368" s="3"/>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A369" s="17"/>
+    <row r="369" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B369" s="3"/>
+      <c r="C369" s="3"/>
+      <c r="D369" s="3"/>
       <c r="E369" s="3"/>
-      <c r="M369" s="17"/>
-    </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A370" s="17"/>
+      <c r="F369" s="3"/>
+      <c r="G369" s="3"/>
+      <c r="H369" s="3"/>
+      <c r="I369" s="3"/>
+      <c r="J369" s="3"/>
+      <c r="K369" s="3"/>
+      <c r="L369" s="3"/>
+    </row>
+    <row r="370" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B370" s="3"/>
+      <c r="C370" s="3"/>
+      <c r="D370" s="3"/>
       <c r="E370" s="3"/>
-      <c r="M370" s="17"/>
-    </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A371" s="17"/>
+      <c r="F370" s="3"/>
+      <c r="G370" s="3"/>
+      <c r="H370" s="3"/>
+      <c r="I370" s="3"/>
+      <c r="J370" s="3"/>
+      <c r="K370" s="3"/>
+      <c r="L370" s="3"/>
+    </row>
+    <row r="371" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B371" s="3"/>
+      <c r="C371" s="3"/>
+      <c r="D371" s="3"/>
       <c r="E371" s="3"/>
-      <c r="M371" s="17"/>
-    </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A372" s="17"/>
+      <c r="F371" s="3"/>
+      <c r="G371" s="3"/>
+      <c r="H371" s="3"/>
+      <c r="I371" s="3"/>
+      <c r="J371" s="3"/>
+      <c r="K371" s="3"/>
+      <c r="L371" s="3"/>
+    </row>
+    <row r="372" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B372" s="3"/>
+      <c r="C372" s="3"/>
+      <c r="D372" s="3"/>
       <c r="E372" s="3"/>
-      <c r="M372" s="17"/>
-    </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A373" s="17"/>
+      <c r="F372" s="3"/>
+      <c r="G372" s="3"/>
+      <c r="H372" s="3"/>
+      <c r="I372" s="3"/>
+      <c r="J372" s="3"/>
+      <c r="K372" s="3"/>
+      <c r="L372" s="3"/>
+    </row>
+    <row r="373" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B373" s="3"/>
+      <c r="C373" s="3"/>
+      <c r="D373" s="3"/>
       <c r="E373" s="3"/>
-      <c r="M373" s="17"/>
-    </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A374" s="17"/>
+      <c r="F373" s="3"/>
+      <c r="G373" s="3"/>
+      <c r="H373" s="3"/>
+      <c r="I373" s="3"/>
+      <c r="J373" s="3"/>
+      <c r="K373" s="3"/>
+      <c r="L373" s="3"/>
+    </row>
+    <row r="374" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B374" s="3"/>
+      <c r="C374" s="3"/>
+      <c r="D374" s="3"/>
       <c r="E374" s="3"/>
-      <c r="M374" s="17"/>
-    </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A375" s="17"/>
+      <c r="F374" s="3"/>
+      <c r="G374" s="3"/>
+      <c r="H374" s="3"/>
+      <c r="I374" s="3"/>
+      <c r="J374" s="3"/>
+      <c r="K374" s="3"/>
+      <c r="L374" s="3"/>
+    </row>
+    <row r="375" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B375" s="3"/>
+      <c r="C375" s="3"/>
+      <c r="D375" s="3"/>
       <c r="E375" s="3"/>
-      <c r="M375" s="17"/>
+      <c r="F375" s="3"/>
+      <c r="G375" s="3"/>
+      <c r="H375" s="3"/>
+      <c r="I375" s="3"/>
+      <c r="J375" s="3"/>
+      <c r="K375" s="3"/>
+      <c r="L375" s="3"/>
+    </row>
+    <row r="376" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B376" s="3"/>
+      <c r="C376" s="3"/>
+      <c r="D376" s="3"/>
+      <c r="E376" s="3"/>
+      <c r="F376" s="3"/>
+      <c r="G376" s="3"/>
+      <c r="H376" s="3"/>
+      <c r="I376" s="3"/>
+      <c r="J376" s="3"/>
+      <c r="K376" s="3"/>
+      <c r="L376" s="3"/>
+    </row>
+    <row r="377" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B377" s="3"/>
+      <c r="C377" s="3"/>
+      <c r="D377" s="3"/>
+      <c r="E377" s="3"/>
+      <c r="F377" s="3"/>
+      <c r="G377" s="3"/>
+      <c r="H377" s="3"/>
+      <c r="I377" s="3"/>
+      <c r="J377" s="3"/>
+      <c r="K377" s="3"/>
+      <c r="L377" s="3"/>
+    </row>
+    <row r="378" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B378" s="3"/>
+      <c r="C378" s="3"/>
+      <c r="D378" s="3"/>
+      <c r="E378" s="3"/>
+      <c r="F378" s="3"/>
+      <c r="G378" s="3"/>
+      <c r="H378" s="3"/>
+      <c r="I378" s="3"/>
+      <c r="J378" s="3"/>
+      <c r="K378" s="3"/>
+      <c r="L378" s="3"/>
+    </row>
+    <row r="379" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B379" s="3"/>
+      <c r="C379" s="3"/>
+      <c r="D379" s="3"/>
+      <c r="E379" s="3"/>
+      <c r="F379" s="3"/>
+      <c r="G379" s="3"/>
+      <c r="H379" s="3"/>
+      <c r="I379" s="3"/>
+      <c r="J379" s="3"/>
+      <c r="K379" s="3"/>
+      <c r="L379" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B89:D89"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B73:D73"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B33:D33"/>
   </mergeCells>
@@ -7837,7 +7974,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few notable additions (for phalanx)
</commit_message>
<xml_diff>
--- a/docs/Comparison.xlsx
+++ b/docs/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\xcom2_my_tweaks\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8762A9-6EC6-4395-A7CD-0293EABA46FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ED4678-04F5-43C5-A1D6-D35A7655754A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6D18C04-5EFF-4A90-9265-84C7107E118D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{B6D18C04-5EFF-4A90-9265-84C7107E118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2047,7 +2047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2201,9 +2201,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2547,8 +2544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A043E2-6980-4E69-B156-F69EB3A846AD}">
   <dimension ref="A1:N385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4892,22 +4889,22 @@
       <c r="E89" s="14" t="s">
         <v>443</v>
       </c>
-      <c r="F89" s="52" t="s">
+      <c r="F89" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="G89" s="52" t="s">
+      <c r="G89" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="H89" s="52" t="s">
+      <c r="H89" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="I89" s="52" t="s">
+      <c r="I89" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="J89" s="52" t="s">
+      <c r="J89" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="K89" s="52" t="s">
+      <c r="K89" s="3" t="s">
         <v>446</v>
       </c>
       <c r="L89" s="3" t="s">

</xml_diff>

<commit_message>
Agent Exclusions and Guardian
</commit_message>
<xml_diff>
--- a/docs/Comparison.xlsx
+++ b/docs/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\xcom2_my_tweaks\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701AA868-C08E-418E-B3F8-8D8F7FBE809A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36B3FF0-6E73-4A7B-9BEF-FD5FE4A705BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{B6D18C04-5EFF-4A90-9265-84C7107E118D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="469">
   <si>
     <t>Comparison</t>
   </si>
@@ -1872,9 +1872,6 @@
     <t>LW2WotC_CloseEncounters</t>
   </si>
   <si>
-    <t>Guard(S)</t>
-  </si>
-  <si>
     <t>DaGuard</t>
   </si>
   <si>
@@ -1888,13 +1885,19 @@
   </si>
   <si>
     <t>MZUnscarred</t>
+  </si>
+  <si>
+    <t>ShadowOps_Inspiration</t>
+  </si>
+  <si>
+    <t>Guardian(S)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2015,6 +2018,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2185,7 +2196,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2366,10 +2377,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2714,8 +2725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A043E2-6980-4E69-B156-F69EB3A846AD}">
   <dimension ref="A1:N389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,7 +3817,7 @@
       <c r="J41" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="K41" s="56" t="s">
         <v>355</v>
       </c>
       <c r="L41" s="3" t="s">
@@ -4408,32 +4419,40 @@
       <c r="L64" s="5"/>
       <c r="M64" s="43"/>
     </row>
-    <row r="65" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>462</v>
+        <v>382</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>463</v>
+        <v>246</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>113</v>
+        <v>331</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>465</v>
+        <v>377</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="G65" s="56" t="s">
-        <v>466</v>
-      </c>
-      <c r="H65" s="56" t="s">
-        <v>467</v>
-      </c>
-      <c r="I65" s="55"/>
-      <c r="J65" s="55"/>
-      <c r="K65" s="55"/>
-      <c r="L65" s="55"/>
+        <v>378</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="I65" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="L65" s="3" t="s">
+        <v>383</v>
+      </c>
       <c r="M65" s="40" t="s">
         <v>376</v>
       </c>
@@ -4452,39 +4471,39 @@
       <c r="L66" s="5"/>
       <c r="M66" s="43"/>
     </row>
-    <row r="67" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>331</v>
+        <v>65</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="I67" s="44" t="s">
-        <v>327</v>
+        <v>372</v>
+      </c>
+      <c r="G67" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H67" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>367</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>381</v>
+        <v>368</v>
+      </c>
+      <c r="K67" s="32" t="s">
+        <v>68</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>383</v>
+        <v>116</v>
       </c>
       <c r="M67" s="40" t="s">
         <v>376</v>
@@ -4504,149 +4523,149 @@
       <c r="L68" s="5"/>
       <c r="M68" s="43"/>
     </row>
-    <row r="69" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="G69" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H69" s="37" t="s">
-        <v>285</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="K69" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="L69" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M69" s="40" t="s">
+    <row r="69" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="26"/>
+      <c r="B69" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="8"/>
+    </row>
+    <row r="70" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="26"/>
+      <c r="B70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M70" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="N70" s="8"/>
+    </row>
+    <row r="71" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I71" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" s="40" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="43"/>
-    </row>
-    <row r="71" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
-      <c r="B71" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="C71" s="53"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="42"/>
-      <c r="N71" s="8"/>
-    </row>
-    <row r="72" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
-      <c r="B72" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K72" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L72" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M72" s="42" t="s">
-        <v>375</v>
-      </c>
-      <c r="N72" s="8"/>
-    </row>
-    <row r="73" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="43"/>
+    </row>
+    <row r="73" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="11" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>282</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>457</v>
+        <v>283</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="I73" s="16" t="s">
         <v>16</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
       <c r="M73" s="40" t="s">
         <v>376</v>
@@ -4666,39 +4685,39 @@
       <c r="L74" s="5"/>
       <c r="M74" s="43"/>
     </row>
-    <row r="75" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
-        <v>143</v>
+    <row r="75" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B75" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>282</v>
+        <v>12</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>283</v>
+        <v>152</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I75" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>146</v>
+        <v>29</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J75" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>144</v>
+        <v>23</v>
       </c>
       <c r="M75" s="40" t="s">
         <v>376</v>
@@ -4718,151 +4737,151 @@
       <c r="L76" s="5"/>
       <c r="M76" s="43"/>
     </row>
-    <row r="77" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B77" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K77" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L77" s="3" t="s">
-        <v>23</v>
-      </c>
+    <row r="77" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="26"/>
+      <c r="B77" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" s="53"/>
+      <c r="D77" s="54"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
       <c r="M77" s="40" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="43"/>
-    </row>
-    <row r="79" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
-      <c r="B79" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="C79" s="53"/>
-      <c r="D79" s="54"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
+      <c r="N77" s="8"/>
+    </row>
+    <row r="78" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="26"/>
+      <c r="B78" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M78" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="N78" s="8"/>
+    </row>
+    <row r="79" spans="1:14" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="M79" s="40" t="s">
         <v>376</v>
       </c>
-      <c r="N79" s="8"/>
-    </row>
-    <row r="80" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E80" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L80" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M80" s="42" t="s">
-        <v>375</v>
-      </c>
-      <c r="N80" s="8"/>
-    </row>
-    <row r="81" spans="2:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="43"/>
+    </row>
+    <row r="81" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="M81" s="40" t="s">
         <v>376</v>
@@ -4882,39 +4901,39 @@
       <c r="L82" s="5"/>
       <c r="M82" s="43"/>
     </row>
-    <row r="83" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="11" t="s">
-        <v>72</v>
+        <v>281</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>73</v>
+        <v>206</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>74</v>
+        <v>336</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K83" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L83" s="3" t="s">
-        <v>82</v>
+        <v>207</v>
+      </c>
+      <c r="F83" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="G83" s="49" t="s">
+        <v>209</v>
+      </c>
+      <c r="H83" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="I83" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="J83" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="K83" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="L83" s="49" t="s">
+        <v>214</v>
       </c>
       <c r="M83" s="40" t="s">
         <v>376</v>
@@ -4934,39 +4953,39 @@
       <c r="L84" s="5"/>
       <c r="M84" s="43"/>
     </row>
-    <row r="85" spans="2:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="11" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>336</v>
+        <v>24</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="F85" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="G85" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="H85" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="I85" s="49" t="s">
-        <v>211</v>
-      </c>
-      <c r="J85" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="K85" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="L85" s="49" t="s">
-        <v>214</v>
+        <v>233</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="M85" s="40" t="s">
         <v>376</v>
@@ -4986,39 +5005,39 @@
       <c r="L86" s="5"/>
       <c r="M86" s="43"/>
     </row>
-    <row r="87" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="11" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>235</v>
+        <v>389</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>235</v>
+        <v>389</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>236</v>
+        <v>390</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>236</v>
+        <v>390</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="M87" s="40" t="s">
         <v>376</v>
@@ -5040,37 +5059,37 @@
     </row>
     <row r="89" spans="2:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="11" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>74</v>
+        <v>280</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>251</v>
+        <v>422</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>252</v>
+        <v>423</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>252</v>
+        <v>424</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>389</v>
+        <v>425</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>389</v>
+        <v>426</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>390</v>
+        <v>428</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="M89" s="40" t="s">
         <v>376</v>
@@ -5090,39 +5109,39 @@
       <c r="L90" s="5"/>
       <c r="M90" s="43"/>
     </row>
-    <row r="91" spans="2:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="11" t="s">
-        <v>277</v>
+        <v>338</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>278</v>
+        <v>201</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>424</v>
+        <v>441</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>426</v>
+        <v>442</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>428</v>
+        <v>443</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>429</v>
+        <v>202</v>
       </c>
       <c r="M91" s="40" t="s">
         <v>376</v>
@@ -5142,39 +5161,39 @@
       <c r="L92" s="5"/>
       <c r="M92" s="43"/>
     </row>
-    <row r="93" spans="2:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="11" t="s">
-        <v>338</v>
+        <v>444</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>201</v>
+        <v>445</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>331</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>202</v>
+        <v>453</v>
       </c>
       <c r="M93" s="40" t="s">
         <v>376</v>
@@ -5194,39 +5213,39 @@
       <c r="L94" s="5"/>
       <c r="M94" s="43"/>
     </row>
-    <row r="95" spans="2:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="11" t="s">
-        <v>444</v>
+        <v>419</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>445</v>
+        <v>420</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>331</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="J95" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="L95" s="3" t="s">
-        <v>453</v>
+        <v>421</v>
+      </c>
+      <c r="F95" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="G95" s="49" t="s">
+        <v>209</v>
+      </c>
+      <c r="H95" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="I95" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="J95" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="K95" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="L95" s="49" t="s">
+        <v>214</v>
       </c>
       <c r="M95" s="40" t="s">
         <v>376</v>
@@ -5246,149 +5265,149 @@
       <c r="L96" s="5"/>
       <c r="M96" s="43"/>
     </row>
-    <row r="97" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E97" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="F97" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="G97" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="H97" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="I97" s="49" t="s">
-        <v>211</v>
-      </c>
-      <c r="J97" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="K97" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="L97" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="M97" s="40" t="s">
+    <row r="97" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="26"/>
+      <c r="B97" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="C97" s="53"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="40"/>
+      <c r="N97" s="8"/>
+    </row>
+    <row r="98" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="26"/>
+      <c r="B98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L98" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M98" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="N98" s="8"/>
+    </row>
+    <row r="99" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="L99" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M99" s="40" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="43"/>
-    </row>
-    <row r="99" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
-      <c r="B99" s="53" t="s">
-        <v>301</v>
-      </c>
-      <c r="C99" s="53"/>
-      <c r="D99" s="54"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
-      <c r="M99" s="40"/>
-      <c r="N99" s="8"/>
-    </row>
-    <row r="100" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
-      <c r="B100" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I100" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K100" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L100" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M100" s="42" t="s">
-        <v>375</v>
-      </c>
-      <c r="N100" s="8"/>
-    </row>
-    <row r="101" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="43"/>
+    </row>
+    <row r="101" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
-        <v>40</v>
+        <v>294</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>388</v>
+        <v>300</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>391</v>
+        <v>296</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>391</v>
+        <v>297</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I101" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>317</v>
+        <v>298</v>
+      </c>
+      <c r="I101" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J101" s="34" t="s">
+        <v>159</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="M101" s="40" t="s">
         <v>376</v>
@@ -5410,37 +5429,37 @@
     </row>
     <row r="103" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
-        <v>294</v>
+        <v>131</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>295</v>
+        <v>139</v>
       </c>
       <c r="D103" s="13" t="s">
         <v>128</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>300</v>
+        <v>132</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>296</v>
+        <v>133</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>297</v>
+        <v>134</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="I103" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J103" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>299</v>
+        <v>135</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K103" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>160</v>
+        <v>303</v>
       </c>
       <c r="M103" s="40" t="s">
         <v>376</v>
@@ -5460,39 +5479,39 @@
       <c r="L104" s="5"/>
       <c r="M104" s="43"/>
     </row>
-    <row r="105" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D105" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E105" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F105" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G105" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>137</v>
+        <v>27</v>
+      </c>
+      <c r="I105" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="K105" s="9" t="s">
-        <v>138</v>
+        <v>21</v>
+      </c>
+      <c r="K105" s="31" t="s">
+        <v>68</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>303</v>
+        <v>22</v>
       </c>
       <c r="M105" s="40" t="s">
         <v>376</v>
@@ -5508,43 +5527,43 @@
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
-      <c r="K106" s="5"/>
+      <c r="K106" s="10"/>
       <c r="L106" s="5"/>
       <c r="M106" s="43"/>
     </row>
-    <row r="107" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>141</v>
+        <v>304</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>140</v>
+        <v>305</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E107" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F107" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="G107" s="35" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G107" s="16" t="s">
+        <v>310</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I107" s="30" t="s">
-        <v>20</v>
+        <v>311</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>307</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K107" s="31" t="s">
-        <v>68</v>
+        <v>306</v>
+      </c>
+      <c r="K107" s="9" t="s">
+        <v>312</v>
       </c>
       <c r="L107" s="3" t="s">
-        <v>22</v>
+        <v>313</v>
       </c>
       <c r="M107" s="40" t="s">
         <v>376</v>
@@ -5564,149 +5583,149 @@
       <c r="L108" s="5"/>
       <c r="M108" s="43"/>
     </row>
-    <row r="109" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="G109" s="3" t="s">
+    <row r="109" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="26"/>
+      <c r="B109" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="C109" s="53"/>
+      <c r="D109" s="54"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="42"/>
+      <c r="N109" s="8"/>
+    </row>
+    <row r="110" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="26"/>
+      <c r="B110" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H110" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I110" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K110" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L110" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M110" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="N110" s="8"/>
+    </row>
+    <row r="111" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E111" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="K111" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="L111" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="M111" s="40" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="5"/>
+      <c r="L112" s="5"/>
+      <c r="M112" s="43"/>
+    </row>
+    <row r="113" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="49" t="s">
+        <v>468</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="I113" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="H109" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="J109" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="K109" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="L109" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="M109" s="40" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="5"/>
-      <c r="I110" s="5"/>
-      <c r="J110" s="5"/>
-      <c r="K110" s="10"/>
-      <c r="L110" s="5"/>
-      <c r="M110" s="43"/>
-    </row>
-    <row r="111" spans="1:14" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
-      <c r="B111" s="53" t="s">
-        <v>238</v>
-      </c>
-      <c r="C111" s="53"/>
-      <c r="D111" s="54"/>
-      <c r="E111" s="21"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="42"/>
-      <c r="N111" s="8"/>
-    </row>
-    <row r="112" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
-      <c r="B112" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E112" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F112" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G112" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I112" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J112" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K112" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L112" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M112" s="42" t="s">
-        <v>375</v>
-      </c>
-      <c r="N112" s="8"/>
-    </row>
-    <row r="113" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E113" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H113" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K113" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="L113" s="3" t="s">
-        <v>199</v>
+      <c r="J113" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="K113" s="56" t="s">
+        <v>355</v>
+      </c>
+      <c r="L113" s="55" t="s">
+        <v>467</v>
       </c>
       <c r="M113" s="40" t="s">
         <v>376</v>
@@ -9582,86 +9601,46 @@
       <c r="L384" s="3"/>
       <c r="M384" s="40"/>
     </row>
-    <row r="385" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A385" s="17"/>
       <c r="B385" s="3"/>
-      <c r="C385" s="3"/>
-      <c r="D385" s="3"/>
       <c r="E385" s="3"/>
-      <c r="F385" s="3"/>
-      <c r="G385" s="3"/>
-      <c r="H385" s="3"/>
-      <c r="I385" s="3"/>
-      <c r="J385" s="3"/>
-      <c r="K385" s="3"/>
-      <c r="L385" s="3"/>
-      <c r="M385" s="40"/>
-    </row>
-    <row r="386" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N385" s="17"/>
+    </row>
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A386" s="17"/>
       <c r="B386" s="3"/>
-      <c r="C386" s="3"/>
-      <c r="D386" s="3"/>
       <c r="E386" s="3"/>
-      <c r="F386" s="3"/>
-      <c r="G386" s="3"/>
-      <c r="H386" s="3"/>
-      <c r="I386" s="3"/>
-      <c r="J386" s="3"/>
-      <c r="K386" s="3"/>
-      <c r="L386" s="3"/>
-      <c r="M386" s="40"/>
-    </row>
-    <row r="387" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N386" s="17"/>
+    </row>
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A387" s="17"/>
       <c r="B387" s="3"/>
-      <c r="C387" s="3"/>
-      <c r="D387" s="3"/>
       <c r="E387" s="3"/>
-      <c r="F387" s="3"/>
-      <c r="G387" s="3"/>
-      <c r="H387" s="3"/>
-      <c r="I387" s="3"/>
-      <c r="J387" s="3"/>
-      <c r="K387" s="3"/>
-      <c r="L387" s="3"/>
-      <c r="M387" s="40"/>
-    </row>
-    <row r="388" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N387" s="17"/>
+    </row>
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A388" s="17"/>
       <c r="B388" s="3"/>
-      <c r="C388" s="3"/>
-      <c r="D388" s="3"/>
       <c r="E388" s="3"/>
-      <c r="F388" s="3"/>
-      <c r="G388" s="3"/>
-      <c r="H388" s="3"/>
-      <c r="I388" s="3"/>
-      <c r="J388" s="3"/>
-      <c r="K388" s="3"/>
-      <c r="L388" s="3"/>
-      <c r="M388" s="40"/>
-    </row>
-    <row r="389" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N388" s="17"/>
+    </row>
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A389" s="17"/>
       <c r="B389" s="3"/>
-      <c r="C389" s="3"/>
-      <c r="D389" s="3"/>
       <c r="E389" s="3"/>
-      <c r="F389" s="3"/>
-      <c r="G389" s="3"/>
-      <c r="H389" s="3"/>
-      <c r="I389" s="3"/>
-      <c r="J389" s="3"/>
-      <c r="K389" s="3"/>
-      <c r="L389" s="3"/>
-      <c r="M389" s="40"/>
+      <c r="N389" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B109:D109"/>
     <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B97:D97"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B77:D77"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B37:D37"/>
   </mergeCells>

</xml_diff>